<commit_message>
add two new vaccine adjuvent per request, issues: https://github.com/vaccineontology/VO/issues/730,https://github.com/vaccineontology/VO/issues/731
</commit_message>
<xml_diff>
--- a/src/vo_new_terms_IDs.xlsx
+++ b/src/vo_new_terms_IDs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurel/Desktop/he lab/VO/src/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezhen/Documents/Ontology/VO/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{799832A7-4DAF-BA49-BF49-0DFB4CCFE2E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23FEC668-537F-C44D-907A-75A39F732CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1300" yWindow="760" windowWidth="28620" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,9 +36,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>vaccine adjuvant</t>
-  </si>
-  <si>
-    <t>VO_0005507 - VO_0005560</t>
   </si>
   <si>
     <t>VO_0005573 - VO_0005599</t>
@@ -74,30 +71,33 @@
     <t>VO:0010373</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
+  <si>
+    <t>VO_0005509 - VO_0005560</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="等线 Light"/>
+      <name val="Aptos Display"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -105,7 +105,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -113,7 +113,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -121,35 +121,35 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF006100"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF9C0006"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF9C5700"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF3F3F76"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -157,7 +157,7 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -165,14 +165,14 @@
       <b/>
       <sz val="12"/>
       <color rgb="FFFA7D00"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFFA7D00"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -180,14 +180,14 @@
       <b/>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -195,7 +195,7 @@
       <i/>
       <sz val="12"/>
       <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -203,14 +203,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -218,7 +218,7 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -226,7 +226,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -234,14 +234,14 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -627,49 +627,49 @@
     </xf>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20% - 着色 1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="42" xr:uid="{FE0908DD-F709-5245-A5EA-61E6D1360987}"/>
-    <cellStyle name="标题" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="标题 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="标题 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="标题 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="标题 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="差" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="好" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="汇总" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="计算" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="检查单元格" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="解释性文本" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="警告文本" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="链接单元格" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="适中" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="输出" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="输入" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="着色 1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="着色 2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="着色 3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="着色 4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="着色 5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -685,7 +685,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1004,232 +1004,232 @@
   <dimension ref="A1:C5531"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.5" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="3" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="3" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="3" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="2" t="s">
-        <v>11</v>
+      <c r="C16" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="7" t="s">
-        <v>10</v>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
+        <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="2" t="s">
+      <c r="C17" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="1"/>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39"/>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40"/>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41"/>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42"/>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43"/>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44"/>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45"/>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46"/>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47"/>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48"/>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49"/>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50"/>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51"/>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52"/>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53"/>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54"/>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55"/>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56"/>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57"/>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58"/>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59"/>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60"/>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61"/>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62"/>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63"/>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64"/>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65"/>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66"/>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67"/>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68"/>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69"/>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70"/>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71"/>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72"/>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73"/>
     </row>
-    <row r="74" spans="1:1">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74"/>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75"/>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76"/>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77"/>
     </row>
-    <row r="78" spans="1:1">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78"/>
     </row>
-    <row r="79" spans="1:1">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79"/>
     </row>
-    <row r="80" spans="1:1">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80"/>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81"/>
     </row>
-    <row r="82" spans="1:1">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82"/>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83"/>
     </row>
-    <row r="84" spans="1:1">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84"/>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85"/>
     </row>
-    <row r="86" spans="1:1">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86"/>
     </row>
-    <row r="87" spans="1:1">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87"/>
     </row>
-    <row r="5460" spans="1:1">
+    <row r="5460" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5460" s="4"/>
     </row>
-    <row r="5518" spans="1:1">
+    <row r="5518" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5518" s="6"/>
     </row>
-    <row r="5531" spans="1:1">
+    <row r="5531" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5531" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new FDA vaccine, and adjuvant
</commit_message>
<xml_diff>
--- a/src/vo_new_terms_IDs.xlsx
+++ b/src/vo_new_terms_IDs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurel/Desktop/he lab/VO/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D69955-D09F-1F47-8F24-680A045B583C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1580980D-B8A3-5E46-9910-A4A0D5B6CEFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1300" yWindow="760" windowWidth="28620" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,7 +71,7 @@
     <t>VO_0005509 - VO_0005560</t>
   </si>
   <si>
-    <t>VO:0010390</t>
+    <t>VO:0010393</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
 </sst>
@@ -1004,7 +1004,7 @@
   <dimension ref="A1:C5531"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
add vaccine monovalent role, vaccine multivalent role
</commit_message>
<xml_diff>
--- a/src/vo_new_terms_IDs.xlsx
+++ b/src/vo_new_terms_IDs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurel/Desktop/he lab/VO/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1580980D-B8A3-5E46-9910-A4A0D5B6CEFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A6F4694-F92E-F946-A268-15EA3E65E6B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1300" yWindow="760" windowWidth="28620" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,7 +71,7 @@
     <t>VO_0005509 - VO_0005560</t>
   </si>
   <si>
-    <t>VO:0010393</t>
+    <t>VO:0010395</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
 </sst>
@@ -1004,7 +1004,7 @@
   <dimension ref="A1:C5531"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
implement flu season property
</commit_message>
<xml_diff>
--- a/src/vo_new_terms_IDs.xlsx
+++ b/src/vo_new_terms_IDs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurel/Desktop/he lab/VO/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A6F4694-F92E-F946-A268-15EA3E65E6B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1D1C63-9953-C642-AE8E-D5EFFA4AE667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1300" yWindow="760" windowWidth="28620" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,7 +71,7 @@
     <t>VO_0005509 - VO_0005560</t>
   </si>
   <si>
-    <t>VO:0010395</t>
+    <t>VO:0010415</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
 </sst>
@@ -1004,7 +1004,7 @@
   <dimension ref="A1:C5531"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
updated base on comments
</commit_message>
<xml_diff>
--- a/src/vo_new_terms_IDs.xlsx
+++ b/src/vo_new_terms_IDs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurel/Desktop/he lab/VO/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1D1C63-9953-C642-AE8E-D5EFFA4AE667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C62860-A1CF-AA46-82A1-456E89CCB868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1300" yWindow="760" windowWidth="28620" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,7 +71,7 @@
     <t>VO_0005509 - VO_0005560</t>
   </si>
   <si>
-    <t>VO:0010415</t>
+    <t>VO:0010434</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
 </sst>
@@ -1004,7 +1004,7 @@
   <dimension ref="A1:C5531"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
clean up 'licensed vaccine role' and its subclasses, add 'authorized vaccine role', and updated licensed/authorized vaccine roles that associated with vaccines
</commit_message>
<xml_diff>
--- a/src/vo_new_terms_IDs.xlsx
+++ b/src/vo_new_terms_IDs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurel/Desktop/he lab/VO/src/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezhen/Documents/Ontology/VO/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C62860-A1CF-AA46-82A1-456E89CCB868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC679B2-A201-EB42-88AD-932BE1BB9097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="760" windowWidth="28620" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="700" yWindow="760" windowWidth="28620" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VO IDs range" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>vaccine adjuvant</t>
   </si>
@@ -73,31 +73,52 @@
   <si>
     <t>VO:0010434</t>
     <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>VO:0007745</t>
+  </si>
+  <si>
+    <t>VO:0007746</t>
+  </si>
+  <si>
+    <t>Simian immunodeficiency virus protein</t>
+  </si>
+  <si>
+    <t>Topografov virus protein</t>
+  </si>
+  <si>
+    <t>Pseudomonas aeruginosa protein</t>
+  </si>
+  <si>
+    <t>Reserved IDs</t>
+  </si>
+  <si>
+    <t>VO:0007750</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="等线 Light"/>
+      <name val="Aptos Display"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -105,7 +126,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -113,7 +134,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -121,35 +142,35 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF006100"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF9C0006"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF9C5700"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF3F3F76"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -157,7 +178,7 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -165,14 +186,14 @@
       <b/>
       <sz val="12"/>
       <color rgb="FFFA7D00"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFFA7D00"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -180,14 +201,14 @@
       <b/>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -195,7 +216,7 @@
       <i/>
       <sz val="12"/>
       <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -203,14 +224,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -218,7 +239,7 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -226,7 +247,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -234,15 +255,33 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="等线"/>
-      <family val="2"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -612,7 +651,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -625,51 +664,57 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20% - 着色 1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="42" xr:uid="{FE0908DD-F709-5245-A5EA-61E6D1360987}"/>
-    <cellStyle name="标题" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="标题 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="标题 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="标题 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="标题 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="差" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="好" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="汇总" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="计算" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="检查单元格" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="解释性文本" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="警告文本" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="链接单元格" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="适中" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="输出" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="输入" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="着色 1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="着色 2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="着色 3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="着色 4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="着色 5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -685,7 +730,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1003,64 +1048,72 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C5531"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.5" style="3" customWidth="1"/>
+    <col min="1" max="1" width="51.33203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="11"/>
+      <c r="C10" s="10"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B11" s="11"/>
+      <c r="C11" s="10"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>4</v>
       </c>
@@ -1068,7 +1121,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>8</v>
       </c>
@@ -1076,160 +1129,189 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39"/>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40"/>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41"/>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42"/>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43"/>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44"/>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45"/>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46"/>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47"/>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48"/>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49"/>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50"/>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51"/>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52"/>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53"/>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54"/>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55"/>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56"/>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57"/>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58"/>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59"/>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60"/>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61"/>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62"/>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63"/>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64"/>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65"/>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66"/>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67"/>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68"/>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69"/>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70"/>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71"/>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72"/>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73"/>
     </row>
-    <row r="74" spans="1:1">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74"/>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75"/>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76"/>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77"/>
     </row>
-    <row r="78" spans="1:1">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78"/>
     </row>
-    <row r="79" spans="1:1">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79"/>
     </row>
-    <row r="80" spans="1:1">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80"/>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81"/>
     </row>
-    <row r="82" spans="1:1">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82"/>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83"/>
     </row>
-    <row r="84" spans="1:1">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84"/>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85"/>
     </row>
-    <row r="86" spans="1:1">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86"/>
     </row>
-    <row r="87" spans="1:1">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87"/>
     </row>
-    <row r="5460" spans="1:1">
+    <row r="5460" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5460" s="4"/>
     </row>
-    <row r="5518" spans="1:1">
+    <row r="5518" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5518" s="6"/>
     </row>
-    <row r="5531" spans="1:1">
+    <row r="5531" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5531" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add 'IL-12-MOP (CTX-1796)' vaccine adjuvant, issue:https://github.com/vaccineontology/VO/issues/740
</commit_message>
<xml_diff>
--- a/src/vo_new_terms_IDs.xlsx
+++ b/src/vo_new_terms_IDs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezhen/Documents/Ontology/VO/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC679B2-A201-EB42-88AD-932BE1BB9097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8052D119-E28C-1349-B898-16F5F0F0A623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="700" yWindow="760" windowWidth="28620" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7660" yWindow="2060" windowWidth="28620" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VO IDs range" sheetId="2" r:id="rId1"/>
@@ -68,9 +68,6 @@
     <t>reserve for cancer vaccine (VO_0007000 - VO_0008999)</t>
   </si>
   <si>
-    <t>VO_0005509 - VO_0005560</t>
-  </si>
-  <si>
     <t>VO:0010434</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
@@ -94,6 +91,9 @@
   </si>
   <si>
     <t>VO:0007750</t>
+  </si>
+  <si>
+    <t>VO_0005510 - VO_0005560</t>
   </si>
 </sst>
 </file>
@@ -651,7 +651,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -665,10 +665,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
@@ -1048,8 +1046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C5531"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1064,7 +1062,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1089,7 +1087,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1107,7 +1105,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1130,32 +1128,32 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="11" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B23" s="10" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added vaccine against pathogen/disease intermediate terms, and updated CVX code mappings
</commit_message>
<xml_diff>
--- a/src/vo_new_terms_IDs.xlsx
+++ b/src/vo_new_terms_IDs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezhen/Documents/Ontology/VO/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8052D119-E28C-1349-B898-16F5F0F0A623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{023EAA9C-DBA2-C44E-A52E-CCD7688F8046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7660" yWindow="2060" windowWidth="28620" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="680" yWindow="5000" windowWidth="28620" windowHeight="13000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VO IDs range" sheetId="2" r:id="rId1"/>
@@ -68,10 +68,6 @@
     <t>reserve for cancer vaccine (VO_0007000 - VO_0008999)</t>
   </si>
   <si>
-    <t>VO:0010434</t>
-    <phoneticPr fontId="21" type="noConversion"/>
-  </si>
-  <si>
     <t>VO:0007745</t>
   </si>
   <si>
@@ -94,6 +90,9 @@
   </si>
   <si>
     <t>VO_0005510 - VO_0005560</t>
+  </si>
+  <si>
+    <t>VO:0010458</t>
   </si>
 </sst>
 </file>
@@ -1047,7 +1046,7 @@
   <dimension ref="A1:C5531"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1062,7 +1061,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1087,7 +1086,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1105,7 +1104,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1129,7 +1128,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -1137,23 +1136,23 @@
         <v>9</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add COVID-19 XBB.1.5 vaccines
</commit_message>
<xml_diff>
--- a/src/vo_new_terms_IDs.xlsx
+++ b/src/vo_new_terms_IDs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezhen/Documents/Ontology/VO/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{023EAA9C-DBA2-C44E-A52E-CCD7688F8046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5297EE77-6729-3A4D-8592-2DC20F0464BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="5000" windowWidth="28620" windowHeight="13000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="540" yWindow="1360" windowWidth="28620" windowHeight="13000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VO IDs range" sheetId="2" r:id="rId1"/>
@@ -59,9 +59,6 @@
     <t>RxNorm Term starting from</t>
   </si>
   <si>
-    <t>VO:0021167</t>
-  </si>
-  <si>
     <t>VO:0007744</t>
   </si>
   <si>
@@ -92,7 +89,10 @@
     <t>VO_0005510 - VO_0005560</t>
   </si>
   <si>
-    <t>VO:0010458</t>
+    <t>VO:0010461</t>
+  </si>
+  <si>
+    <t>VO:0021180</t>
   </si>
 </sst>
 </file>
@@ -1046,7 +1046,7 @@
   <dimension ref="A1:C5531"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1061,7 +1061,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1081,12 +1081,12 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1104,7 +1104,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1120,7 +1120,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
@@ -1128,31 +1128,31 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add two new vaccine adjuvants, issues: https://github.com/vaccineontology/VO/issues/759,https://github.com/vaccineontology/VO/issues/760
</commit_message>
<xml_diff>
--- a/src/vo_new_terms_IDs.xlsx
+++ b/src/vo_new_terms_IDs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezhen/Documents/Ontology/VO/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5297EE77-6729-3A4D-8592-2DC20F0464BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B21B2C-7FE4-B54A-A5F7-681768D00CF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="1360" windowWidth="28620" windowHeight="13000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7260" yWindow="1580" windowWidth="28620" windowHeight="13000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VO IDs range" sheetId="2" r:id="rId1"/>
@@ -86,13 +86,13 @@
     <t>VO:0007750</t>
   </si>
   <si>
-    <t>VO_0005510 - VO_0005560</t>
-  </si>
-  <si>
     <t>VO:0010461</t>
   </si>
   <si>
     <t>VO:0021180</t>
+  </si>
+  <si>
+    <t>VO_0005512 - VO_0005560</t>
   </si>
 </sst>
 </file>
@@ -1046,7 +1046,7 @@
   <dimension ref="A1:C5531"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1061,7 +1061,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1104,7 +1104,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1120,7 +1120,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
deprecated 3 terms, issues:https://github.com/vaccineontology/VO/issues/768,https://github.com/vaccineontology/VO/issues/80,https://github.com/vaccineontology/VO/issues/543, fixed wrong parent of VO:0010155, issue: https://github.com/vaccineontology/VO/issues/767; add new term 'Fluzone High-Dose 2010-2011 vaccine', issue: https://github.com/vaccineontology/VO/issues/766
</commit_message>
<xml_diff>
--- a/src/vo_new_terms_IDs.xlsx
+++ b/src/vo_new_terms_IDs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezhen/Documents/Ontology/VO/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B21B2C-7FE4-B54A-A5F7-681768D00CF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0947995-8C5D-434F-9A6E-C725A440B8A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7260" yWindow="1580" windowWidth="28620" windowHeight="13000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1620" yWindow="1580" windowWidth="28620" windowHeight="13000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VO IDs range" sheetId="2" r:id="rId1"/>
@@ -89,10 +89,10 @@
     <t>VO:0010461</t>
   </si>
   <si>
-    <t>VO:0021180</t>
-  </si>
-  <si>
     <t>VO_0005512 - VO_0005560</t>
+  </si>
+  <si>
+    <t>VO:0021181</t>
   </si>
 </sst>
 </file>
@@ -1045,8 +1045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C5531"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1061,7 +1061,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1120,7 +1120,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
add two new vaccine-induced response terms and reorganize vaccine-induced response related terms
</commit_message>
<xml_diff>
--- a/src/vo_new_terms_IDs.xlsx
+++ b/src/vo_new_terms_IDs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezhen/Documents/Ontology/VO/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0947995-8C5D-434F-9A6E-C725A440B8A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{853BF3D2-E59A-354C-A5AE-6C2402178E0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1620" yWindow="1580" windowWidth="28620" windowHeight="13000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -86,13 +86,13 @@
     <t>VO:0007750</t>
   </si>
   <si>
-    <t>VO:0010461</t>
-  </si>
-  <si>
     <t>VO_0005512 - VO_0005560</t>
   </si>
   <si>
     <t>VO:0021181</t>
+  </si>
+  <si>
+    <t>VO:0010463</t>
   </si>
 </sst>
 </file>
@@ -1045,8 +1045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C5531"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1061,7 +1061,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1104,7 +1104,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1120,7 +1120,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
add two kinds of immune biomarker
</commit_message>
<xml_diff>
--- a/src/vo_new_terms_IDs.xlsx
+++ b/src/vo_new_terms_IDs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezhen/Documents/Ontology/VO/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{853BF3D2-E59A-354C-A5AE-6C2402178E0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F626F88A-D2F7-0143-9DAC-E685CAA50859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="1580" windowWidth="28620" windowHeight="13000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1620" yWindow="3720" windowWidth="28620" windowHeight="13000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VO IDs range" sheetId="2" r:id="rId1"/>
@@ -92,7 +92,7 @@
     <t>VO:0021181</t>
   </si>
   <si>
-    <t>VO:0010463</t>
+    <t>VO:0010465</t>
   </si>
 </sst>
 </file>
@@ -1045,7 +1045,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C5531"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add 3 new vaccine adjuvants, issues: https://github.com/vaccineontology/VO/issues/784,https://github.com/vaccineontology/VO/issues/785,https://github.com/vaccineontology/VO/issues/787
</commit_message>
<xml_diff>
--- a/src/vo_new_terms_IDs.xlsx
+++ b/src/vo_new_terms_IDs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezhen/Documents/Ontology/VO/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F626F88A-D2F7-0143-9DAC-E685CAA50859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{069CD30F-8B34-E54C-A797-C74995FC1C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="3720" windowWidth="28620" windowHeight="13000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8000" yWindow="2840" windowWidth="28620" windowHeight="13000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VO IDs range" sheetId="2" r:id="rId1"/>
@@ -86,13 +86,13 @@
     <t>VO:0007750</t>
   </si>
   <si>
-    <t>VO_0005512 - VO_0005560</t>
-  </si>
-  <si>
     <t>VO:0021181</t>
   </si>
   <si>
     <t>VO:0010465</t>
+  </si>
+  <si>
+    <t>VO_0005515 - VO_0005560</t>
   </si>
 </sst>
 </file>
@@ -1045,8 +1045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C5531"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1061,7 +1061,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1104,7 +1104,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1120,7 +1120,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
update axioms and definitions of three high-level vaccine terms
</commit_message>
<xml_diff>
--- a/src/vo_new_terms_IDs.xlsx
+++ b/src/vo_new_terms_IDs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezhen/Documents/Ontology/VO/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{069CD30F-8B34-E54C-A797-C74995FC1C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39FD247-765E-ED4F-B4C8-E998DAC3EAA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8000" yWindow="2840" windowWidth="28620" windowHeight="13000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1620" yWindow="820" windowWidth="28620" windowHeight="13000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VO IDs range" sheetId="2" r:id="rId1"/>
@@ -89,10 +89,10 @@
     <t>VO:0021181</t>
   </si>
   <si>
-    <t>VO:0010465</t>
-  </si>
-  <si>
     <t>VO_0005515 - VO_0005560</t>
+  </si>
+  <si>
+    <t>VO:0010475</t>
   </si>
 </sst>
 </file>
@@ -1043,10 +1043,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C5531"/>
+  <dimension ref="A1:C5526"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1061,7 +1061,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1104,7 +1104,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1155,6 +1155,21 @@
         <v>14</v>
       </c>
     </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38"/>
+    </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39"/>
     </row>
@@ -1287,33 +1302,18 @@
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A83"/>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A84"/>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A85"/>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A86"/>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A87"/>
-    </row>
-    <row r="5460" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5460" s="4"/>
-    </row>
-    <row r="5518" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5518" s="6"/>
-    </row>
-    <row r="5531" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5531" s="5"/>
+    <row r="5455" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5455" s="4"/>
+    </row>
+    <row r="5513" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5513" s="6"/>
+    </row>
+    <row r="5526" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5526" s="5"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H9:H93">
-    <sortCondition ref="H9:H93"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H9:H88">
+    <sortCondition ref="H9:H88"/>
   </sortState>
   <phoneticPr fontId="21" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update IDs used for new terms
</commit_message>
<xml_diff>
--- a/src/vo_new_terms_IDs.xlsx
+++ b/src/vo_new_terms_IDs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezhen/Documents/Ontology/VO/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39FD247-765E-ED4F-B4C8-E998DAC3EAA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36AAAEDD-86C8-1241-A779-C80A9FDDC41C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="820" windowWidth="28620" windowHeight="13000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1620" yWindow="780" windowWidth="28620" windowHeight="13000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VO IDs range" sheetId="2" r:id="rId1"/>
@@ -92,14 +92,14 @@
     <t>VO_0005515 - VO_0005560</t>
   </si>
   <si>
-    <t>VO:0010475</t>
+    <t>VO:0010492</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -281,6 +281,13 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -660,13 +667,13 @@
     <xf numFmtId="0" fontId="19" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1045,8 +1052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C5526"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1090,12 +1097,12 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="11"/>
-      <c r="C10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="9"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="11"/>
-      <c r="C11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="9"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
@@ -1103,7 +1110,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="13" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1127,31 +1134,31 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="11" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
implemented inactivated vaccine and live attenuated vaccine using vaccine role
</commit_message>
<xml_diff>
--- a/src/vo_new_terms_IDs.xlsx
+++ b/src/vo_new_terms_IDs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezhen/Documents/Ontology/VO/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36AAAEDD-86C8-1241-A779-C80A9FDDC41C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC6CB2C-7C03-CA4B-95DB-78F6958F91BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="780" windowWidth="28620" windowHeight="13000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="180" yWindow="900" windowWidth="28620" windowHeight="13000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VO IDs range" sheetId="2" r:id="rId1"/>
@@ -33,14 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="269">
   <si>
     <t>vaccine adjuvant</t>
   </si>
   <si>
-    <t>VO_0005573 - VO_0005599</t>
-  </si>
-  <si>
     <t>VO_0005814 - VO_0005999</t>
   </si>
   <si>
@@ -89,17 +86,767 @@
     <t>VO:0021181</t>
   </si>
   <si>
-    <t>VO_0005515 - VO_0005560</t>
-  </si>
-  <si>
     <t>VO:0010492</t>
+  </si>
+  <si>
+    <t>VO_0005515</t>
+  </si>
+  <si>
+    <t>VO_0005516</t>
+  </si>
+  <si>
+    <t>VO_0005517</t>
+  </si>
+  <si>
+    <t>VO_0005518</t>
+  </si>
+  <si>
+    <t>VO_0005520</t>
+  </si>
+  <si>
+    <t>VO_0005521</t>
+  </si>
+  <si>
+    <t>VO_0005522</t>
+  </si>
+  <si>
+    <t>VO_0005523</t>
+  </si>
+  <si>
+    <t>VO_0005524</t>
+  </si>
+  <si>
+    <t>VO_0005525</t>
+  </si>
+  <si>
+    <t>VO_0005526</t>
+  </si>
+  <si>
+    <t>VO_0005527</t>
+  </si>
+  <si>
+    <t>VO_0005528</t>
+  </si>
+  <si>
+    <t>VO_0005529</t>
+  </si>
+  <si>
+    <t>VO_0005530</t>
+  </si>
+  <si>
+    <t>VO_0005531</t>
+  </si>
+  <si>
+    <t>VO_0005532</t>
+  </si>
+  <si>
+    <t>VO_0005533</t>
+  </si>
+  <si>
+    <t>VO_0005534</t>
+  </si>
+  <si>
+    <t>VO_0005535</t>
+  </si>
+  <si>
+    <t>VO_0005536</t>
+  </si>
+  <si>
+    <t>VO_0005537</t>
+  </si>
+  <si>
+    <t>VO_0005538</t>
+  </si>
+  <si>
+    <t>VO_0005539</t>
+  </si>
+  <si>
+    <t>VO_0005540</t>
+  </si>
+  <si>
+    <t>VO_0005541</t>
+  </si>
+  <si>
+    <t>VO_0005542</t>
+  </si>
+  <si>
+    <t>VO_0005543</t>
+  </si>
+  <si>
+    <t>VO_0005544</t>
+  </si>
+  <si>
+    <t>VO_0005545</t>
+  </si>
+  <si>
+    <t>VO_0005546</t>
+  </si>
+  <si>
+    <t>VO_0005547</t>
+  </si>
+  <si>
+    <t>VO_0005548</t>
+  </si>
+  <si>
+    <t>VO_0005549</t>
+  </si>
+  <si>
+    <t>VO_0005550</t>
+  </si>
+  <si>
+    <t>VO_0005551</t>
+  </si>
+  <si>
+    <t>VO_0005552</t>
+  </si>
+  <si>
+    <t>VO_0005553</t>
+  </si>
+  <si>
+    <t>VO_0005554</t>
+  </si>
+  <si>
+    <t>VO_0005555</t>
+  </si>
+  <si>
+    <t>VO_0005556</t>
+  </si>
+  <si>
+    <t>VO_0005557</t>
+  </si>
+  <si>
+    <t>VO_0005558</t>
+  </si>
+  <si>
+    <t>VO_0005559</t>
+  </si>
+  <si>
+    <t>VO_0005560</t>
+  </si>
+  <si>
+    <t>VO_0005573</t>
+  </si>
+  <si>
+    <t>VO_0005574</t>
+  </si>
+  <si>
+    <t>VO_0005575</t>
+  </si>
+  <si>
+    <t>VO_0005576</t>
+  </si>
+  <si>
+    <t>VO_0005577</t>
+  </si>
+  <si>
+    <t>VO_0005578</t>
+  </si>
+  <si>
+    <t>VO_0005579</t>
+  </si>
+  <si>
+    <t>VO_0005580</t>
+  </si>
+  <si>
+    <t>VO_0005581</t>
+  </si>
+  <si>
+    <t>VO_0005582</t>
+  </si>
+  <si>
+    <t>VO_0005583</t>
+  </si>
+  <si>
+    <t>VO_0005584</t>
+  </si>
+  <si>
+    <t>VO_0005585</t>
+  </si>
+  <si>
+    <t>VO_0005586</t>
+  </si>
+  <si>
+    <t>VO_0005587</t>
+  </si>
+  <si>
+    <t>VO_0005588</t>
+  </si>
+  <si>
+    <t>VO_0005589</t>
+  </si>
+  <si>
+    <t>VO_0005590</t>
+  </si>
+  <si>
+    <t>VO_0005591</t>
+  </si>
+  <si>
+    <t>VO_0005592</t>
+  </si>
+  <si>
+    <t>VO_0005593</t>
+  </si>
+  <si>
+    <t>VO_0005594</t>
+  </si>
+  <si>
+    <t>VO_0005595</t>
+  </si>
+  <si>
+    <t>VO_0005596</t>
+  </si>
+  <si>
+    <t>VO_0005597</t>
+  </si>
+  <si>
+    <t>VO_0005598</t>
+  </si>
+  <si>
+    <t>VO_0005599</t>
+  </si>
+  <si>
+    <t>VO_0005600</t>
+  </si>
+  <si>
+    <t>VO_0005601</t>
+  </si>
+  <si>
+    <t>VO_0005602</t>
+  </si>
+  <si>
+    <t>VO_0005603</t>
+  </si>
+  <si>
+    <t>VO_0005604</t>
+  </si>
+  <si>
+    <t>VO_0005605</t>
+  </si>
+  <si>
+    <t>VO_0005606</t>
+  </si>
+  <si>
+    <t>VO_0005607</t>
+  </si>
+  <si>
+    <t>VO_0005608</t>
+  </si>
+  <si>
+    <t>VO_0005609</t>
+  </si>
+  <si>
+    <t>VO_0005610</t>
+  </si>
+  <si>
+    <t>VO_0005611</t>
+  </si>
+  <si>
+    <t>VO_0005612</t>
+  </si>
+  <si>
+    <t>VO_0005613</t>
+  </si>
+  <si>
+    <t>VO_0005614</t>
+  </si>
+  <si>
+    <t>VO_0005615</t>
+  </si>
+  <si>
+    <t>VO_0005616</t>
+  </si>
+  <si>
+    <t>VO_0005617</t>
+  </si>
+  <si>
+    <t>VO_0005618</t>
+  </si>
+  <si>
+    <t>VO_0005619</t>
+  </si>
+  <si>
+    <t>VO_0005620</t>
+  </si>
+  <si>
+    <t>VO_0005621</t>
+  </si>
+  <si>
+    <t>VO_0005622</t>
+  </si>
+  <si>
+    <t>VO_0005623</t>
+  </si>
+  <si>
+    <t>VO_0005624</t>
+  </si>
+  <si>
+    <t>VO_0005625</t>
+  </si>
+  <si>
+    <t>VO_0005626</t>
+  </si>
+  <si>
+    <t>VO_0005627</t>
+  </si>
+  <si>
+    <t>VO_0005628</t>
+  </si>
+  <si>
+    <t>VO_0005629</t>
+  </si>
+  <si>
+    <t>VO_0005630</t>
+  </si>
+  <si>
+    <t>VO_0005631</t>
+  </si>
+  <si>
+    <t>VO_0005632</t>
+  </si>
+  <si>
+    <t>VO_0005633</t>
+  </si>
+  <si>
+    <t>VO_0005634</t>
+  </si>
+  <si>
+    <t>VO_0005635</t>
+  </si>
+  <si>
+    <t>VO_0005636</t>
+  </si>
+  <si>
+    <t>VO_0005637</t>
+  </si>
+  <si>
+    <t>VO_0005638</t>
+  </si>
+  <si>
+    <t>VO_0005639</t>
+  </si>
+  <si>
+    <t>VO_0005640</t>
+  </si>
+  <si>
+    <t>VO_0005641</t>
+  </si>
+  <si>
+    <t>VO_0005642</t>
+  </si>
+  <si>
+    <t>VO_0005643</t>
+  </si>
+  <si>
+    <t>VO_0005644</t>
+  </si>
+  <si>
+    <t>VO_0005645</t>
+  </si>
+  <si>
+    <t>VO_0005646</t>
+  </si>
+  <si>
+    <t>VO_0005647</t>
+  </si>
+  <si>
+    <t>VO_0005648</t>
+  </si>
+  <si>
+    <t>VO_0005649</t>
+  </si>
+  <si>
+    <t>VO_0005650</t>
+  </si>
+  <si>
+    <t>VO_0005651</t>
+  </si>
+  <si>
+    <t>VO_0005652</t>
+  </si>
+  <si>
+    <t>VO_0005653</t>
+  </si>
+  <si>
+    <t>VO_0005654</t>
+  </si>
+  <si>
+    <t>VO_0005655</t>
+  </si>
+  <si>
+    <t>VO_0005656</t>
+  </si>
+  <si>
+    <t>VO_0005657</t>
+  </si>
+  <si>
+    <t>VO_0005658</t>
+  </si>
+  <si>
+    <t>VO_0005659</t>
+  </si>
+  <si>
+    <t>VO_0005660</t>
+  </si>
+  <si>
+    <t>VO_0005661</t>
+  </si>
+  <si>
+    <t>VO_0005662</t>
+  </si>
+  <si>
+    <t>VO_0005663</t>
+  </si>
+  <si>
+    <t>VO_0005664</t>
+  </si>
+  <si>
+    <t>VO_0005665</t>
+  </si>
+  <si>
+    <t>VO_0005666</t>
+  </si>
+  <si>
+    <t>VO_0005667</t>
+  </si>
+  <si>
+    <t>VO_0005668</t>
+  </si>
+  <si>
+    <t>VO_0005669</t>
+  </si>
+  <si>
+    <t>VO_0005670</t>
+  </si>
+  <si>
+    <t>VO_0005671</t>
+  </si>
+  <si>
+    <t>VO_0005672</t>
+  </si>
+  <si>
+    <t>VO_0005673</t>
+  </si>
+  <si>
+    <t>VO_0005674</t>
+  </si>
+  <si>
+    <t>VO_0005675</t>
+  </si>
+  <si>
+    <t>VO_0005676</t>
+  </si>
+  <si>
+    <t>VO_0005677</t>
+  </si>
+  <si>
+    <t>VO_0005678</t>
+  </si>
+  <si>
+    <t>VO_0005679</t>
+  </si>
+  <si>
+    <t>VO_0005680</t>
+  </si>
+  <si>
+    <t>VO_0005681</t>
+  </si>
+  <si>
+    <t>VO_0005682</t>
+  </si>
+  <si>
+    <t>VO_0005683</t>
+  </si>
+  <si>
+    <t>VO_0005684</t>
+  </si>
+  <si>
+    <t>VO_0005685</t>
+  </si>
+  <si>
+    <t>VO_0005686</t>
+  </si>
+  <si>
+    <t>VO_0005687</t>
+  </si>
+  <si>
+    <t>VO_0005688</t>
+  </si>
+  <si>
+    <t>VO_0005689</t>
+  </si>
+  <si>
+    <t>VO_0005690</t>
+  </si>
+  <si>
+    <t>VO_0005691</t>
+  </si>
+  <si>
+    <t>VO_0005692</t>
+  </si>
+  <si>
+    <t>VO_0005693</t>
+  </si>
+  <si>
+    <t>VO_0005694</t>
+  </si>
+  <si>
+    <t>VO_0005695</t>
+  </si>
+  <si>
+    <t>VO_0005696</t>
+  </si>
+  <si>
+    <t>VO_0005697</t>
+  </si>
+  <si>
+    <t>VO_0005698</t>
+  </si>
+  <si>
+    <t>VO_0005699</t>
+  </si>
+  <si>
+    <t>VO_0005700</t>
+  </si>
+  <si>
+    <t>VO_0005701</t>
+  </si>
+  <si>
+    <t>VO_0005702</t>
+  </si>
+  <si>
+    <t>VO_0005703</t>
+  </si>
+  <si>
+    <t>VO_0005704</t>
+  </si>
+  <si>
+    <t>VO_0005705</t>
+  </si>
+  <si>
+    <t>VO_0005706</t>
+  </si>
+  <si>
+    <t>VO_0005707</t>
+  </si>
+  <si>
+    <t>VO_0005708</t>
+  </si>
+  <si>
+    <t>VO_0005709</t>
+  </si>
+  <si>
+    <t>VO_0005710</t>
+  </si>
+  <si>
+    <t>VO_0005711</t>
+  </si>
+  <si>
+    <t>VO_0005712</t>
+  </si>
+  <si>
+    <t>VO_0005713</t>
+  </si>
+  <si>
+    <t>VO_0005714</t>
+  </si>
+  <si>
+    <t>VO_0005715</t>
+  </si>
+  <si>
+    <t>VO_0005716</t>
+  </si>
+  <si>
+    <t>VO_0005717</t>
+  </si>
+  <si>
+    <t>VO_0005718</t>
+  </si>
+  <si>
+    <t>VO_0005719</t>
+  </si>
+  <si>
+    <t>VO_0005720</t>
+  </si>
+  <si>
+    <t>VO_0005721</t>
+  </si>
+  <si>
+    <t>VO_0005722</t>
+  </si>
+  <si>
+    <t>VO_0005723</t>
+  </si>
+  <si>
+    <t>VO_0005724</t>
+  </si>
+  <si>
+    <t>VO_0005725</t>
+  </si>
+  <si>
+    <t>VO_0005726</t>
+  </si>
+  <si>
+    <t>VO_0005727</t>
+  </si>
+  <si>
+    <t>VO_0005728</t>
+  </si>
+  <si>
+    <t>VO_0005729</t>
+  </si>
+  <si>
+    <t>VO_0005730</t>
+  </si>
+  <si>
+    <t>VO_0005731</t>
+  </si>
+  <si>
+    <t>VO_0005732</t>
+  </si>
+  <si>
+    <t>VO_0005733</t>
+  </si>
+  <si>
+    <t>VO_0005734</t>
+  </si>
+  <si>
+    <t>VO_0005735</t>
+  </si>
+  <si>
+    <t>VO_0005736</t>
+  </si>
+  <si>
+    <t>VO_0005737</t>
+  </si>
+  <si>
+    <t>VO_0005738</t>
+  </si>
+  <si>
+    <t>VO_0005739</t>
+  </si>
+  <si>
+    <t>VO_0005740</t>
+  </si>
+  <si>
+    <t>VO_0005741</t>
+  </si>
+  <si>
+    <t>VO_0005742</t>
+  </si>
+  <si>
+    <t>VO_0005743</t>
+  </si>
+  <si>
+    <t>VO_0005744</t>
+  </si>
+  <si>
+    <t>VO_0005745</t>
+  </si>
+  <si>
+    <t>VO_0005746</t>
+  </si>
+  <si>
+    <t>VO_0005747</t>
+  </si>
+  <si>
+    <t>VO_0005748</t>
+  </si>
+  <si>
+    <t>VO_0005749</t>
+  </si>
+  <si>
+    <t>VO_0005750</t>
+  </si>
+  <si>
+    <t>VO_0005751</t>
+  </si>
+  <si>
+    <t>VO_0005752</t>
+  </si>
+  <si>
+    <t>VO_0005753</t>
+  </si>
+  <si>
+    <t>VO_0005754</t>
+  </si>
+  <si>
+    <t>VO_0005755</t>
+  </si>
+  <si>
+    <t>VO_0005756</t>
+  </si>
+  <si>
+    <t>VO_0005757</t>
+  </si>
+  <si>
+    <t>VO_0005758</t>
+  </si>
+  <si>
+    <t>VO_0005759</t>
+  </si>
+  <si>
+    <t>VO_0005760</t>
+  </si>
+  <si>
+    <t>VO_0005761</t>
+  </si>
+  <si>
+    <t>VO_0005762</t>
+  </si>
+  <si>
+    <t>VO_0005763</t>
+  </si>
+  <si>
+    <t>VO_0005764</t>
+  </si>
+  <si>
+    <t>VO_0005765</t>
+  </si>
+  <si>
+    <t>VO_0005766</t>
+  </si>
+  <si>
+    <t>VO_0005767</t>
+  </si>
+  <si>
+    <t>VO_0005768</t>
+  </si>
+  <si>
+    <t>VO_0005769</t>
+  </si>
+  <si>
+    <t>VO_0005770</t>
+  </si>
+  <si>
+    <t>VO_0005771</t>
+  </si>
+  <si>
+    <t>VO_0005772</t>
+  </si>
+  <si>
+    <t>VO_0005773</t>
+  </si>
+  <si>
+    <t>VO_0005774</t>
+  </si>
+  <si>
+    <t>ID assigned to ajuvants that will be added to VO</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets/d/1HelnswxZv1ConGKWusuEO6XzDLe9hjEog1ejSiVOQhs/edit?gid=1705240071#gid=1705240071</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Detail see: </t>
+  </si>
+  <si>
+    <t>VO_0005775 - VO_0005799</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -290,6 +1037,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="37">
     <fill>
@@ -612,7 +1367,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -656,8 +1411,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -674,8 +1430,10 @@
     <xf numFmtId="0" fontId="25" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="43"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -709,6 +1467,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1050,264 +1809,1375 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C5526"/>
+  <dimension ref="A1:H5526"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="51.33203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>265</v>
+      </c>
+      <c r="H1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="G2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H2" s="15" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="G8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="G9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B10" s="10"/>
       <c r="C10" s="9"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B11" s="10"/>
       <c r="C11" s="9"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="G15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="G17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
-        <v>8</v>
-      </c>
       <c r="B21" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="11" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
+      <c r="G22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B23" s="9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G32" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G33" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G35" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G36" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G37" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G38" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G39" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40"/>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G40" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41"/>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G41" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42"/>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G42" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43"/>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G43" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44"/>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G44" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45"/>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G45" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46"/>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G46" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47"/>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G47" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G48" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49"/>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G49" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50"/>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G50" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51"/>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G51" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52"/>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G52" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53"/>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G53" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54"/>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G54" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55"/>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G55" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56"/>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G56" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57"/>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G57" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58"/>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G58" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59"/>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G59" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60"/>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G60" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61"/>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G61" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62"/>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G62" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63"/>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G63" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64"/>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G64" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65"/>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G65" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66"/>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G66" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67"/>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G67" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68"/>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G68" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69"/>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G69" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70"/>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G70" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71"/>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G71" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72"/>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G72" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73"/>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G73" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74"/>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G74" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75"/>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G75" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76"/>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G76" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77"/>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G77" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78"/>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G78" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79"/>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G79" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80"/>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G80" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81"/>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G81" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82"/>
+      <c r="G82" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G83" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G84" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G85" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G86" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G87" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G88" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G89" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G90" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G91" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G92" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G93" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G94" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G95" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G96" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="97" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G97" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="98" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G98" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="99" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G99" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="100" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G100" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="101" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G101" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="102" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G102" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="103" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G103" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="104" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G104" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="105" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G105" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="106" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G106" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="107" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G107" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="108" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G108" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="109" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G109" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="110" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G110" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="111" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G111" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="112" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G112" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="113" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G113" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="114" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G114" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="115" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G115" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="116" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G116" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="117" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G117" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="118" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G118" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="119" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G119" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="120" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G120" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="121" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G121" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="122" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G122" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="123" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G123" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="124" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G124" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="125" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G125" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="126" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G126" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="127" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G127" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="128" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G128" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="129" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G129" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="130" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G130" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="131" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G131" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="132" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G132" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="133" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G133" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="134" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G134" t="s">
+        <v>150</v>
+      </c>
+      <c r="H134" s="14"/>
+    </row>
+    <row r="135" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G135" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="136" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G136" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="137" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G137" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="138" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G138" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="139" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G139" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="140" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G140" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="141" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G141" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="142" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G142" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="143" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G143" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="144" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G144" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="145" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G145" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="146" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G146" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="147" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G147" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="148" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G148" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="149" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G149" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="150" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G150" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="151" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G151" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="152" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G152" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="153" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G153" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="154" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G154" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="155" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G155" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="156" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G156" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="157" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G157" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="158" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G158" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="159" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G159" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="160" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G160" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="161" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G161" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="162" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G162" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="163" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G163" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="164" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G164" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="165" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G165" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="166" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G166" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="167" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G167" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="168" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G168" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="169" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G169" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="170" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G170" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="171" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G171" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="172" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G172" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="173" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G173" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="174" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G174" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="175" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G175" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="176" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G176" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="177" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G177" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="178" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G178" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="179" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G179" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="180" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G180" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="181" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G181" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="182" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G182" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="183" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G183" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="184" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G184" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="185" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G185" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="186" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G186" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="187" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G187" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="188" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G188" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="189" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G189" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="190" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G190" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="191" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G191" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="192" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G192" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="193" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G193" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="194" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G194" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="195" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G195" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="196" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G196" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="197" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G197" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="198" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G198" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="199" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G199" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="200" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G200" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="201" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G201" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="202" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G202" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="203" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G203" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="204" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G204" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="205" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G205" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="206" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G206" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="207" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G207" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="208" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G208" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="209" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G209" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="210" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G210" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="211" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G211" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="212" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G212" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="213" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G213" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="214" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G214" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="215" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G215" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="216" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G216" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="217" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G217" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="218" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G218" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="219" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G219" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="220" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G220" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="221" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G221" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="222" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G222" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="223" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G223" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="224" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G224" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="225" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G225" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="226" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G226" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="227" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G227" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="228" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G228" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="229" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G229" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="230" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G230" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="231" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G231" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="232" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G232" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="233" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G233" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="234" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G234" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="235" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G235" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="236" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G236" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="237" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G237" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="238" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G238" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="239" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G239" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="240" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G240" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="241" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G241" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="242" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G242" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="243" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G243" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="244" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G244" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="245" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G245" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="246" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G246" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="247" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G247" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="248" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G248" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="5455" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5455" s="4"/>
@@ -1319,10 +3189,13 @@
       <c r="A5526" s="5"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H9:H88">
-    <sortCondition ref="H9:H88"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G1:G5526">
+    <sortCondition ref="G1:G5526"/>
   </sortState>
   <phoneticPr fontId="21" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" location="gid=1705240071" xr:uid="{9A45402F-F49A-7A46-9FDB-BC4722C03E51}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
reserve VO IDs for adjuvants
</commit_message>
<xml_diff>
--- a/src/vo_new_terms_IDs.xlsx
+++ b/src/vo_new_terms_IDs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezhen/Documents/Ontology/VO/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC6CB2C-7C03-CA4B-95DB-78F6958F91BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A32EC04-293C-D544-91A8-D80B0D666869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="900" windowWidth="28620" windowHeight="13000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5680" yWindow="900" windowWidth="28620" windowHeight="13000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VO IDs range" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="294">
   <si>
     <t>vaccine adjuvant</t>
   </si>
@@ -839,7 +839,82 @@
     <t xml:space="preserve">Detail see: </t>
   </si>
   <si>
-    <t>VO_0005775 - VO_0005799</t>
+    <t>VO_0005775</t>
+  </si>
+  <si>
+    <t>VO_0005776</t>
+  </si>
+  <si>
+    <t>VO_0005777</t>
+  </si>
+  <si>
+    <t>VO_0005778</t>
+  </si>
+  <si>
+    <t>VO_0005779</t>
+  </si>
+  <si>
+    <t>VO_0005780</t>
+  </si>
+  <si>
+    <t>VO_0005781</t>
+  </si>
+  <si>
+    <t>VO_0005782</t>
+  </si>
+  <si>
+    <t>LT-IIb</t>
+  </si>
+  <si>
+    <t>PI-sRI</t>
+  </si>
+  <si>
+    <t>2GO53</t>
+  </si>
+  <si>
+    <t>MSP-102</t>
+  </si>
+  <si>
+    <t>HBsAg</t>
+  </si>
+  <si>
+    <t>7DW8-5</t>
+  </si>
+  <si>
+    <t>CTA2B</t>
+  </si>
+  <si>
+    <t>PI-RI</t>
+  </si>
+  <si>
+    <t>https://violinet.org/vaxjo/vaxjo_detail.php?c_vaxjo_id=110</t>
+  </si>
+  <si>
+    <t>https://violinet.org/vaxjo/vaxjo_detail.php?c_vaxjo_id=185</t>
+  </si>
+  <si>
+    <t>https://violinet.org/vaxjo/vaxjo_detail.php?c_vaxjo_id=139</t>
+  </si>
+  <si>
+    <t>https://violinet.org/vaxjo/vaxjo_detail.php?c_vaxjo_id=178</t>
+  </si>
+  <si>
+    <t>https://violinet.org/vaxjo/vaxjo_detail.php?c_vaxjo_id=136</t>
+  </si>
+  <si>
+    <t>https://violinet.org/vaxjo/vaxjo_detail.php?c_vaxjo_id=143</t>
+  </si>
+  <si>
+    <t>https://violinet.org/vaxjo/vaxjo_detail.php?c_vaxjo_id=111</t>
+  </si>
+  <si>
+    <t>https://violinet.org/vaxjo/vaxjo_detail.php?c_vaxjo_id=184</t>
+  </si>
+  <si>
+    <t>Vaxjo adjuvants need to be added</t>
+  </si>
+  <si>
+    <t>VO_0005783 - VO_0005799</t>
   </si>
 </sst>
 </file>
@@ -1809,10 +1884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H5526"/>
+  <dimension ref="A1:I5526"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A159" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1834,7 +1909,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>268</v>
+        <v>293</v>
       </c>
       <c r="G2" t="s">
         <v>18</v>
@@ -3139,44 +3214,135 @@
         <v>256</v>
       </c>
     </row>
-    <row r="241" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="241" spans="4:9" x14ac:dyDescent="0.2">
       <c r="G241" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="242" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="242" spans="4:9" x14ac:dyDescent="0.2">
       <c r="G242" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="243" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="243" spans="4:9" x14ac:dyDescent="0.2">
       <c r="G243" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="244" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="244" spans="4:9" x14ac:dyDescent="0.2">
       <c r="G244" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="245" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="245" spans="4:9" x14ac:dyDescent="0.2">
       <c r="G245" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="246" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="246" spans="4:9" x14ac:dyDescent="0.2">
       <c r="G246" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="247" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="247" spans="4:9" x14ac:dyDescent="0.2">
       <c r="G247" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="248" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="248" spans="4:9" x14ac:dyDescent="0.2">
       <c r="G248" t="s">
         <v>264</v>
+      </c>
+    </row>
+    <row r="249" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D249" t="s">
+        <v>292</v>
+      </c>
+      <c r="G249" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="H249" t="s">
+        <v>276</v>
+      </c>
+      <c r="I249" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="250" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="G250" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="H250" t="s">
+        <v>277</v>
+      </c>
+      <c r="I250" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="251" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="G251" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="H251" t="s">
+        <v>278</v>
+      </c>
+      <c r="I251" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="252" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="G252" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="H252" t="s">
+        <v>279</v>
+      </c>
+      <c r="I252" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="253" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="G253" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="H253" t="s">
+        <v>280</v>
+      </c>
+      <c r="I253" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="254" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="G254" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="H254" t="s">
+        <v>281</v>
+      </c>
+      <c r="I254" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="255" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="G255" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="H255" t="s">
+        <v>282</v>
+      </c>
+      <c r="I255" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="256" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="G256" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="H256" t="s">
+        <v>283</v>
+      </c>
+      <c r="I256" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="5455" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update available new term IDs
</commit_message>
<xml_diff>
--- a/src/vo_new_terms_IDs.xlsx
+++ b/src/vo_new_terms_IDs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezhen/Documents/Ontology/VO/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A32EC04-293C-D544-91A8-D80B0D666869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{236B9D86-41E7-5447-AB5F-57EC0D84F889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5680" yWindow="900" windowWidth="28620" windowHeight="13000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9800" yWindow="3860" windowWidth="28620" windowHeight="13000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VO IDs range" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="302">
   <si>
     <t>vaccine adjuvant</t>
   </si>
@@ -86,9 +86,6 @@
     <t>VO:0021181</t>
   </si>
   <si>
-    <t>VO:0010492</t>
-  </si>
-  <si>
     <t>VO_0005515</t>
   </si>
   <si>
@@ -915,13 +912,40 @@
   </si>
   <si>
     <t>VO_0005783 - VO_0005799</t>
+  </si>
+  <si>
+    <t>VO_0005783</t>
+  </si>
+  <si>
+    <t>VO_0005784</t>
+  </si>
+  <si>
+    <t>TLR agonist vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>plant-derived vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>VO_0005785</t>
+  </si>
+  <si>
+    <t>VO_0005786</t>
+  </si>
+  <si>
+    <t>7DW8-5 vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>AS15 vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>VO:0010493</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1120,8 +1144,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="5"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1325,8 +1368,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1441,6 +1490,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1488,7 +1552,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1507,6 +1571,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="43"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1886,8 +1955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I5526"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A159" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1901,21 +1970,21 @@
         <v>0</v>
       </c>
       <c r="G1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -1923,7 +1992,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1931,22 +2000,22 @@
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1954,7 +2023,7 @@
         <v>8</v>
       </c>
       <c r="G8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -1962,21 +2031,21 @@
         <v>15</v>
       </c>
       <c r="G9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B10" s="10"/>
       <c r="C10" s="9"/>
       <c r="G10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B11" s="10"/>
       <c r="C11" s="9"/>
       <c r="G11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -1984,26 +2053,26 @@
         <v>4</v>
       </c>
       <c r="G12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>17</v>
+        <v>301</v>
       </c>
       <c r="G13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="G15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -2014,7 +2083,7 @@
         <v>6</v>
       </c>
       <c r="G16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -2025,17 +2094,17 @@
         <v>5</v>
       </c>
       <c r="G17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -2043,7 +2112,7 @@
         <v>14</v>
       </c>
       <c r="G20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -2054,7 +2123,7 @@
         <v>11</v>
       </c>
       <c r="G21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -2065,7 +2134,7 @@
         <v>12</v>
       </c>
       <c r="G22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -2076,1273 +2145,1305 @@
         <v>13</v>
       </c>
       <c r="G23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34"/>
       <c r="G34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35"/>
       <c r="G35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36"/>
       <c r="G36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37"/>
       <c r="G37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38"/>
       <c r="G38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39"/>
       <c r="G39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40"/>
       <c r="G40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41"/>
       <c r="G41" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42"/>
       <c r="G42" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43"/>
       <c r="G43" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44"/>
       <c r="G44" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45"/>
       <c r="G45" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46"/>
       <c r="G46" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47"/>
       <c r="G47" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48"/>
       <c r="G48" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49"/>
       <c r="G49" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50"/>
       <c r="G50" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51"/>
       <c r="G51" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52"/>
       <c r="G52" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53"/>
       <c r="G53" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54"/>
       <c r="G54" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55"/>
       <c r="G55" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56"/>
       <c r="G56" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57"/>
       <c r="G57" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58"/>
       <c r="G58" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59"/>
       <c r="G59" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60"/>
       <c r="G60" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61"/>
       <c r="G61" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62"/>
       <c r="G62" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63"/>
       <c r="G63" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64"/>
       <c r="G64" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65"/>
       <c r="G65" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66"/>
       <c r="G66" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67"/>
       <c r="G67" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68"/>
       <c r="G68" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69"/>
       <c r="G69" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70"/>
       <c r="G70" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71"/>
       <c r="G71" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72"/>
       <c r="G72" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73"/>
       <c r="G73" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74"/>
       <c r="G74" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75"/>
       <c r="G75" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76"/>
       <c r="G76" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77"/>
       <c r="G77" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78"/>
       <c r="G78" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79"/>
       <c r="G79" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80"/>
       <c r="G80" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81"/>
       <c r="G81" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82"/>
       <c r="G82" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G83" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G84" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G85" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G86" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G87" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G88" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G89" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G90" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G91" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G92" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G93" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G94" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G95" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G96" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="97" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G97" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="98" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G98" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="99" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G99" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="100" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G100" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="101" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G101" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="102" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G102" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="103" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G103" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="104" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G104" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="105" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G105" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="106" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G106" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="107" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G107" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="108" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G108" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="109" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G109" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="110" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G110" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="111" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G111" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="112" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G112" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="113" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G113" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="114" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G114" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="115" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G115" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="116" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G116" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="117" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G117" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="118" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G118" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="119" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G119" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="120" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G120" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="121" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G121" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="122" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G122" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="123" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G123" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="124" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G124" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="125" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G125" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="126" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G126" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="127" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G127" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="128" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G128" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="129" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G129" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="130" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G130" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="131" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G131" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="132" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G132" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="133" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G133" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="134" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G134" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H134" s="14"/>
     </row>
     <row r="135" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G135" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="136" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G136" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="137" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G137" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="138" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G138" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="139" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G139" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="140" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G140" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="141" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G141" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="142" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G142" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="143" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G143" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="144" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G144" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="145" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G145" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="146" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G146" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="147" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G147" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="148" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G148" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="149" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G149" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="150" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G150" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="151" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G151" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="152" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G152" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="153" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G153" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="154" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G154" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="155" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G155" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="156" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G156" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="157" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G157" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="158" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G158" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="159" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G159" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="160" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G160" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="161" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G161" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="162" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G162" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="163" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G163" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="164" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G164" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="165" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G165" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="166" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G166" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="167" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G167" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="168" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G168" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="169" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G169" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="170" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G170" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="171" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G171" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="172" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G172" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="173" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G173" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="174" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G174" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="175" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G175" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="176" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G176" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="177" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G177" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="178" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G178" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="179" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G179" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="180" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G180" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="181" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G181" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="182" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G182" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="183" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G183" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="184" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G184" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="185" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G185" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="186" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G186" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="187" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G187" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="188" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G188" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="189" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G189" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="190" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G190" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="191" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G191" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="192" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G192" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="193" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G193" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="194" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G194" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="195" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G195" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="196" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G196" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="197" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G197" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="198" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G198" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="199" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G199" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="200" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G200" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="201" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G201" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="202" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G202" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="203" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G203" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="204" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G204" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="205" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G205" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="206" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G206" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="207" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G207" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="208" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G208" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="209" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G209" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="210" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G210" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="211" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G211" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="212" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G212" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="213" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G213" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="214" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G214" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="215" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G215" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="216" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G216" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="217" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G217" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="218" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G218" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="219" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G219" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="220" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G220" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="221" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G221" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="222" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G222" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="223" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G223" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="224" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G224" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="225" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G225" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="226" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G226" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="227" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G227" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="228" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G228" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="229" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G229" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="230" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G230" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="231" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G231" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="232" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G232" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="233" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G233" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="234" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G234" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="235" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G235" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="236" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G236" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="237" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G237" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="238" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G238" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="239" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G239" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="240" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G240" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="241" spans="4:9" x14ac:dyDescent="0.2">
       <c r="G241" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="242" spans="4:9" x14ac:dyDescent="0.2">
       <c r="G242" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="243" spans="4:9" x14ac:dyDescent="0.2">
       <c r="G243" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="244" spans="4:9" x14ac:dyDescent="0.2">
       <c r="G244" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="245" spans="4:9" x14ac:dyDescent="0.2">
       <c r="G245" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="246" spans="4:9" x14ac:dyDescent="0.2">
       <c r="G246" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="247" spans="4:9" x14ac:dyDescent="0.2">
       <c r="G247" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="248" spans="4:9" x14ac:dyDescent="0.2">
       <c r="G248" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="249" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D249" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G249" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H249" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I249" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="250" spans="4:9" x14ac:dyDescent="0.2">
       <c r="G250" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H250" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I250" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="251" spans="4:9" x14ac:dyDescent="0.2">
       <c r="G251" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H251" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I251" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="252" spans="4:9" x14ac:dyDescent="0.2">
       <c r="G252" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H252" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I252" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="253" spans="4:9" x14ac:dyDescent="0.2">
       <c r="G253" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H253" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I253" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="254" spans="4:9" x14ac:dyDescent="0.2">
       <c r="G254" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H254" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I254" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="255" spans="4:9" x14ac:dyDescent="0.2">
       <c r="G255" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H255" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I255" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="256" spans="4:9" x14ac:dyDescent="0.2">
       <c r="G256" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="H256" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="I256" t="s">
-        <v>291</v>
+        <v>290</v>
+      </c>
+    </row>
+    <row r="257" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G257" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="H257" s="16" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="258" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G258" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="H258" s="17" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="259" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G259" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="H259" s="18" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="260" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G260" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="H260" s="18" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="5455" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add few new immune profiles
</commit_message>
<xml_diff>
--- a/src/vo_new_terms_IDs.xlsx
+++ b/src/vo_new_terms_IDs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezhen/Documents/Ontology/VO/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{236B9D86-41E7-5447-AB5F-57EC0D84F889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B256B01-9395-7043-A57D-B0F019BB54C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9800" yWindow="3860" windowWidth="28620" windowHeight="13000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -938,7 +938,7 @@
     <t>AS15 vaccine adjuvant</t>
   </si>
   <si>
-    <t>VO:0010493</t>
+    <t>VO:0010503</t>
   </si>
 </sst>
 </file>
@@ -1955,7 +1955,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I5526"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
assigned IDs to newly add vaccine adjuvants after release
</commit_message>
<xml_diff>
--- a/src/vo_new_terms_IDs.xlsx
+++ b/src/vo_new_terms_IDs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezhen/Documents/Ontology/VO/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC452D96-C71C-3743-B863-E938EFD48A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDAC9EF3-80AA-8048-9ABC-3D68CEC2CCFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="2580" windowWidth="28620" windowHeight="13000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10240" yWindow="2060" windowWidth="20680" windowHeight="13000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VO IDs range" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="529">
   <si>
     <t>vaccine adjuvant</t>
   </si>
@@ -1115,9 +1115,6 @@
     <t>IFN-beta vaccine adjuvant</t>
   </si>
   <si>
-    <t>IL-15 vaccine adjuvant</t>
-  </si>
-  <si>
     <t>IL-18 vaccine adjuvant</t>
   </si>
   <si>
@@ -1442,98 +1439,194 @@
     <t>LCP vaccine adjuvant</t>
   </si>
   <si>
-    <t>AAHS vaccine adjuvant</t>
-  </si>
-  <si>
     <t>Ad-p53 vaccine adjuvant</t>
   </si>
   <si>
     <t>Ad-SLC vaccine adjuvant</t>
   </si>
   <si>
-    <t>Alum-TLR7 vaccine adjuvant</t>
-  </si>
-  <si>
     <t>AS1517499 vaccine adjuvant</t>
   </si>
   <si>
-    <t>Cationic adjuvant formulation (CAF) vaccine adjuvant</t>
-  </si>
-  <si>
-    <t>delta-inulin vaccine adjuvant</t>
-  </si>
-  <si>
-    <t>Injectable Excipients vaccine adjuvant</t>
-  </si>
-  <si>
     <t>L. polysaccharide vaccine adjuvant</t>
   </si>
   <si>
-    <t>LAG-3 vaccine adjuvant</t>
-  </si>
-  <si>
-    <t>LT Oral adjuvant vaccine adjuvant</t>
-  </si>
-  <si>
-    <t>Melatonin vaccine adjuvant</t>
-  </si>
-  <si>
-    <t>metformin vaccine adjuvant</t>
-  </si>
-  <si>
     <t>NS-TLR vaccine adjuvant</t>
   </si>
   <si>
-    <t>PCL and chitosan NPs vaccine adjuvant</t>
-  </si>
-  <si>
-    <t>PRR agonists vaccine adjuvant</t>
-  </si>
-  <si>
-    <t>R848 and IL-4 vaccine adjuvant</t>
-  </si>
-  <si>
-    <t>saponin and MPLA nanoparticle vaccine adjuvant</t>
-  </si>
-  <si>
     <t>SBAS2 vaccine adjuvant</t>
   </si>
   <si>
-    <t>Sphingosine-1-phosphate vaccine adjuvant</t>
-  </si>
-  <si>
-    <t>TBK1 vaccine adjuvant</t>
-  </si>
-  <si>
-    <t>TLR ligand liposome vaccine adjuvant</t>
-  </si>
-  <si>
-    <t>TLR3 vaccine adjuvant</t>
-  </si>
-  <si>
-    <t>TLR4 agonist lipopolysaccharide vaccine adjuvant</t>
-  </si>
-  <si>
-    <t>TLR5 vaccine adjuvant</t>
-  </si>
-  <si>
-    <t>TLR7 and TLR8 agonist vaccine adjuvant</t>
-  </si>
-  <si>
-    <t>TLR9 vaccine adjuvant</t>
-  </si>
-  <si>
-    <t>TLRa vaccine adjuvant</t>
-  </si>
-  <si>
-    <t>VO_0005765 - VO_0005799</t>
+    <t>VO:0005519</t>
+  </si>
+  <si>
+    <t>TLR1 agonist vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>TLR2 agonist vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>TLR3 agonist vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>TLR4 agonist vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>TLR5 agonist vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>TLR6 agonist vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>TLR7 agonist vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>TLR8 agonist vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>TLR9 agonist vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>VO:0005765</t>
+  </si>
+  <si>
+    <t>VO:0005766</t>
+  </si>
+  <si>
+    <t>VO:0005767</t>
+  </si>
+  <si>
+    <t>VO:0005768</t>
+  </si>
+  <si>
+    <t>VO:0005769</t>
+  </si>
+  <si>
+    <t>VO:0005770</t>
+  </si>
+  <si>
+    <t>VO:0005771</t>
+  </si>
+  <si>
+    <t>VO:0005772</t>
+  </si>
+  <si>
+    <t>VO:0005773</t>
+  </si>
+  <si>
+    <t>VO:0005774</t>
+  </si>
+  <si>
+    <t>VO:0005775</t>
+  </si>
+  <si>
+    <t>VO:0005776</t>
+  </si>
+  <si>
+    <t>VO:0005777</t>
+  </si>
+  <si>
+    <t>TFPR1 vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>Murabutide vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>Ace-DEX vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>GDQ vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>NADA vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>SMQ vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>PHAD vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>ST101036 vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>MIP-1alpha vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>Levamisole vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>Hsp65 vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>HVJ-Envelope vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>GPI-0100 vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>Tween 80 vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>EP67 vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>1Z105 vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>Curdlan vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>CARP-1 vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>ASPPR vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>BLP vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>BX795 vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>C5a vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>HP-β-CD vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>CYT387 vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>CARP-2 vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>peptide vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>animal-derived vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>VO:0005778</t>
+  </si>
+  <si>
+    <t>fusion protein vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>VO:0005779</t>
+  </si>
+  <si>
+    <t>adenovirus-mediated vaccine adjuvant</t>
+  </si>
+  <si>
+    <t>VO_0005780 - VO_0005799</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1751,8 +1844,29 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="38">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1956,14 +2070,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -2080,17 +2188,30 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -2141,7 +2262,7 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2158,19 +2279,21 @@
     <xf numFmtId="0" fontId="25" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="43"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="44" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="44" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2549,10 +2672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K5526"/>
+  <dimension ref="A1:I5526"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A224" workbookViewId="0">
-      <selection activeCell="G242" sqref="G242"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2575,15 +2698,15 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>497</v>
-      </c>
-      <c r="G2" t="s">
+        <v>528</v>
+      </c>
+      <c r="G2" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="14" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2591,10 +2714,10 @@
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="19" t="s">
         <v>263</v>
       </c>
       <c r="I3" t="s">
@@ -2605,116 +2728,116 @@
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="H4" s="19" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="G5" t="s">
+      <c r="G5" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="19" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="G6" t="s">
+      <c r="G6" s="20" t="s">
+        <v>474</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G7" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="16" t="s">
+      <c r="H7" s="19" t="s">
         <v>266</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="G7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" s="16" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G8" t="s">
-        <v>31</v>
-      </c>
-      <c r="H8" s="16" t="s">
-        <v>268</v>
+      <c r="G8" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G9" t="s">
-        <v>32</v>
-      </c>
-      <c r="H9" s="16" t="s">
-        <v>269</v>
+      <c r="G9" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="19" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B10" s="10"/>
       <c r="C10" s="9"/>
-      <c r="G10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" s="16" t="s">
-        <v>270</v>
+      <c r="G10" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="19" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B11" s="10"/>
       <c r="C11" s="9"/>
-      <c r="G11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H11" s="16" t="s">
-        <v>271</v>
+      <c r="G11" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="19" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G12" t="s">
-        <v>35</v>
-      </c>
-      <c r="H12" s="16" t="s">
-        <v>272</v>
+      <c r="G12" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" s="19" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G14" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="H14" s="19" t="s">
         <v>273</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="G14" t="s">
-        <v>37</v>
-      </c>
-      <c r="H14" s="16" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
-      <c r="G15" t="s">
-        <v>38</v>
-      </c>
-      <c r="H15" s="16" t="s">
-        <v>275</v>
+      <c r="G15" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="19" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -2724,11 +2847,11 @@
       <c r="C16" t="s">
         <v>6</v>
       </c>
-      <c r="G16" t="s">
-        <v>39</v>
-      </c>
-      <c r="H16" s="16" t="s">
-        <v>276</v>
+      <c r="G16" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="H16" s="19" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -2738,38 +2861,38 @@
       <c r="C17" t="s">
         <v>5</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="H17" s="19" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G18" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="H17" s="16" t="s">
+      <c r="H18" s="19" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G18" t="s">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G19" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="H18" s="16" t="s">
+      <c r="H19" s="19" t="s">
         <v>278</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G19" t="s">
-        <v>42</v>
-      </c>
-      <c r="H19" s="16" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G20" t="s">
-        <v>43</v>
-      </c>
-      <c r="H20" s="16" t="s">
-        <v>280</v>
+      <c r="G20" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="H20" s="19" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -2779,11 +2902,11 @@
       <c r="B21" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G21" t="s">
-        <v>44</v>
-      </c>
-      <c r="H21" s="16" t="s">
-        <v>281</v>
+      <c r="G21" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H21" s="19" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -2793,11 +2916,11 @@
       <c r="B22" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G22" t="s">
-        <v>45</v>
-      </c>
-      <c r="H22" s="16" t="s">
-        <v>282</v>
+      <c r="G22" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="H22" s="19" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -2807,2039 +2930,2027 @@
       <c r="B23" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H23" s="19" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G24" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="H23" s="16" t="s">
+      <c r="H24" s="19" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G24" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G25" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="H24" s="16" t="s">
+      <c r="H25" s="19" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G25" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G26" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="H25" s="16" t="s">
+      <c r="H26" s="19" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G26" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G27" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="H26" s="16" t="s">
+      <c r="H27" s="19" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G27" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G28" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="H27" s="16" t="s">
+      <c r="H28" s="19" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G28" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G29" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="H28" s="16" t="s">
+      <c r="H29" s="19" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G29" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G30" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H29" s="16" t="s">
+      <c r="H30" s="19" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G30" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G31" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="H30" s="16" t="s">
+      <c r="H31" s="19" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G31" t="s">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G32" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="H31" s="16" t="s">
+      <c r="H32" s="19" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G32" t="s">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G33" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="H32" s="16" t="s">
+      <c r="H33" s="19" t="s">
         <v>292</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G33" t="s">
-        <v>56</v>
-      </c>
-      <c r="H33" s="16" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34"/>
-      <c r="G34" t="s">
-        <v>57</v>
-      </c>
-      <c r="H34" s="16" t="s">
-        <v>294</v>
+      <c r="G34" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="H34" s="19" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35"/>
-      <c r="G35" t="s">
-        <v>58</v>
-      </c>
-      <c r="H35" s="16" t="s">
-        <v>295</v>
+      <c r="G35" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="H35" s="19" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36"/>
-      <c r="G36" t="s">
-        <v>59</v>
-      </c>
-      <c r="H36" s="16" t="s">
-        <v>296</v>
+      <c r="G36" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="H36" s="19" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37"/>
-      <c r="G37" t="s">
-        <v>60</v>
-      </c>
-      <c r="H37" s="16" t="s">
-        <v>297</v>
+      <c r="G37" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="H37" s="19" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38"/>
-      <c r="G38" t="s">
-        <v>61</v>
-      </c>
-      <c r="H38" s="16" t="s">
-        <v>298</v>
+      <c r="G38" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="H38" s="19" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39"/>
-      <c r="G39" t="s">
-        <v>62</v>
-      </c>
-      <c r="H39" s="16" t="s">
-        <v>299</v>
+      <c r="G39" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="H39" s="19" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40"/>
-      <c r="G40" t="s">
-        <v>63</v>
-      </c>
-      <c r="H40" s="16" t="s">
-        <v>300</v>
+      <c r="G40" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="H40" s="19" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41"/>
-      <c r="G41" t="s">
-        <v>64</v>
-      </c>
-      <c r="H41" s="16" t="s">
-        <v>301</v>
+      <c r="G41" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="H41" s="19" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42"/>
-      <c r="G42" t="s">
-        <v>65</v>
-      </c>
-      <c r="H42" s="16" t="s">
-        <v>302</v>
+      <c r="G42" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="H42" s="19" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43"/>
-      <c r="G43" t="s">
-        <v>66</v>
-      </c>
-      <c r="H43" s="16" t="s">
-        <v>303</v>
+      <c r="G43" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="H43" s="19" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44"/>
-      <c r="G44" t="s">
-        <v>67</v>
-      </c>
-      <c r="H44" s="16" t="s">
-        <v>304</v>
+      <c r="G44" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="H44" s="19" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45"/>
-      <c r="G45" t="s">
-        <v>68</v>
-      </c>
-      <c r="H45" s="16" t="s">
-        <v>305</v>
+      <c r="G45" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="H45" s="19" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46"/>
-      <c r="G46" t="s">
-        <v>69</v>
-      </c>
-      <c r="H46" s="16" t="s">
-        <v>306</v>
+      <c r="G46" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="H46" s="19" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47"/>
-      <c r="G47" t="s">
-        <v>70</v>
-      </c>
-      <c r="H47" s="16" t="s">
-        <v>307</v>
+      <c r="G47" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="H47" s="19" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48"/>
-      <c r="G48" t="s">
-        <v>71</v>
-      </c>
-      <c r="H48" s="16" t="s">
-        <v>308</v>
+      <c r="G48" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="H48" s="19" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49"/>
-      <c r="G49" t="s">
-        <v>72</v>
-      </c>
-      <c r="H49" s="16" t="s">
-        <v>309</v>
+      <c r="G49" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="H49" s="19" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50"/>
-      <c r="G50" t="s">
-        <v>73</v>
-      </c>
-      <c r="H50" s="16" t="s">
-        <v>310</v>
+      <c r="G50" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="H50" s="19" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51"/>
-      <c r="G51" t="s">
-        <v>74</v>
-      </c>
-      <c r="H51" s="16" t="s">
-        <v>311</v>
+      <c r="G51" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="H51" s="19" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52"/>
-      <c r="G52" t="s">
-        <v>75</v>
-      </c>
-      <c r="H52" s="16" t="s">
-        <v>312</v>
+      <c r="G52" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="H52" s="19" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53"/>
-      <c r="G53" t="s">
-        <v>76</v>
-      </c>
-      <c r="H53" s="16" t="s">
-        <v>313</v>
+      <c r="G53" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="H53" s="19" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54"/>
-      <c r="G54" t="s">
-        <v>77</v>
-      </c>
-      <c r="H54" s="16" t="s">
-        <v>314</v>
+      <c r="G54" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="H54" s="19" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55"/>
-      <c r="G55" t="s">
-        <v>78</v>
-      </c>
-      <c r="H55" s="16" t="s">
-        <v>315</v>
+      <c r="G55" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="H55" s="19" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56"/>
-      <c r="G56" t="s">
-        <v>79</v>
-      </c>
-      <c r="H56" s="16" t="s">
-        <v>316</v>
+      <c r="G56" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="H56" s="19" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57"/>
-      <c r="G57" t="s">
-        <v>80</v>
-      </c>
-      <c r="H57" s="16" t="s">
-        <v>317</v>
+      <c r="G57" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="H57" s="19" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58"/>
-      <c r="G58" t="s">
-        <v>81</v>
-      </c>
-      <c r="H58" s="16" t="s">
-        <v>318</v>
+      <c r="G58" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="H58" s="19" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59"/>
-      <c r="G59" t="s">
-        <v>82</v>
-      </c>
-      <c r="H59" s="16" t="s">
-        <v>319</v>
+      <c r="G59" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="H59" s="19" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60"/>
-      <c r="G60" t="s">
-        <v>83</v>
-      </c>
-      <c r="H60" s="16" t="s">
-        <v>320</v>
+      <c r="G60" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="H60" s="19" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61"/>
-      <c r="G61" t="s">
-        <v>84</v>
-      </c>
-      <c r="H61" s="16" t="s">
-        <v>321</v>
+      <c r="G61" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="H61" s="19" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62"/>
-      <c r="G62" t="s">
-        <v>85</v>
-      </c>
-      <c r="H62" s="16" t="s">
-        <v>322</v>
+      <c r="G62" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="H62" s="19" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63"/>
-      <c r="G63" t="s">
-        <v>86</v>
-      </c>
-      <c r="H63" s="16" t="s">
-        <v>323</v>
+      <c r="G63" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="H63" s="19" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64"/>
-      <c r="G64" t="s">
-        <v>87</v>
-      </c>
-      <c r="H64" s="16" t="s">
-        <v>324</v>
+      <c r="G64" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="H64" s="19" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65"/>
-      <c r="G65" t="s">
-        <v>88</v>
-      </c>
-      <c r="H65" s="16" t="s">
-        <v>325</v>
+      <c r="G65" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="H65" s="19" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66"/>
-      <c r="G66" t="s">
-        <v>89</v>
-      </c>
-      <c r="H66" s="16" t="s">
-        <v>326</v>
+      <c r="G66" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="H66" s="19" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67"/>
-      <c r="G67" t="s">
-        <v>90</v>
-      </c>
-      <c r="H67" s="16" t="s">
-        <v>327</v>
+      <c r="G67" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="H67" s="19" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68"/>
-      <c r="G68" t="s">
-        <v>91</v>
-      </c>
-      <c r="H68" s="16" t="s">
-        <v>328</v>
+      <c r="G68" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="H68" s="19" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69"/>
-      <c r="G69" t="s">
-        <v>92</v>
-      </c>
-      <c r="H69" s="16" t="s">
-        <v>329</v>
+      <c r="G69" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="H69" s="19" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70"/>
-      <c r="G70" t="s">
-        <v>93</v>
-      </c>
-      <c r="H70" s="16" t="s">
-        <v>330</v>
+      <c r="G70" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="H70" s="19" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71"/>
-      <c r="G71" t="s">
-        <v>94</v>
-      </c>
-      <c r="H71" s="16" t="s">
-        <v>331</v>
+      <c r="G71" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="H71" s="19" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72"/>
-      <c r="G72" t="s">
-        <v>95</v>
-      </c>
-      <c r="H72" s="16" t="s">
-        <v>332</v>
+      <c r="G72" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="H72" s="19" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73"/>
-      <c r="G73" t="s">
-        <v>96</v>
-      </c>
-      <c r="H73" s="16" t="s">
-        <v>333</v>
+      <c r="G73" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="H73" s="19" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74"/>
-      <c r="G74" t="s">
-        <v>97</v>
-      </c>
-      <c r="H74" s="16" t="s">
-        <v>334</v>
+      <c r="G74" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="H74" s="19" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75"/>
-      <c r="G75" t="s">
-        <v>98</v>
-      </c>
-      <c r="H75" s="16" t="s">
-        <v>335</v>
+      <c r="G75" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="H75" s="19" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76"/>
-      <c r="G76" t="s">
-        <v>99</v>
-      </c>
-      <c r="H76" s="16" t="s">
-        <v>336</v>
+      <c r="G76" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="H76" s="19" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77"/>
-      <c r="G77" t="s">
-        <v>100</v>
-      </c>
-      <c r="H77" s="16" t="s">
-        <v>337</v>
+      <c r="G77" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="H77" s="19" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78"/>
-      <c r="G78" t="s">
-        <v>101</v>
-      </c>
-      <c r="H78" s="16" t="s">
-        <v>338</v>
+      <c r="G78" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="H78" s="19" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79"/>
-      <c r="G79" t="s">
-        <v>102</v>
-      </c>
-      <c r="H79" s="16" t="s">
-        <v>339</v>
+      <c r="G79" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="H79" s="19" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80"/>
-      <c r="G80" t="s">
-        <v>103</v>
-      </c>
-      <c r="H80" s="16" t="s">
-        <v>340</v>
+      <c r="G80" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="H80" s="19" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81"/>
-      <c r="G81" t="s">
-        <v>104</v>
-      </c>
-      <c r="H81" s="16" t="s">
-        <v>341</v>
+      <c r="G81" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="H81" s="19" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82"/>
-      <c r="G82" t="s">
+      <c r="G82" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="H82" s="19" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G83" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="H82" s="16" t="s">
+      <c r="H83" s="19" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G83" t="s">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G84" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="H83" s="16" t="s">
+      <c r="H84" s="19" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G84" t="s">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G85" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="H84" s="16" t="s">
+      <c r="H85" s="19" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G85" t="s">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G86" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="H85" s="16" t="s">
+      <c r="H86" s="19" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G86" t="s">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G87" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="H86" s="16" t="s">
+      <c r="H87" s="19" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G87" t="s">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G88" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="H87" s="16" t="s">
+      <c r="H88" s="19" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G88" t="s">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G89" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="H88" s="16" t="s">
+      <c r="H89" s="19" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G89" t="s">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G90" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="H89" s="16" t="s">
+      <c r="H90" s="19" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G90" t="s">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G91" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="H90" s="16" t="s">
+      <c r="H91" s="19" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G91" t="s">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G92" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="H91" s="16" t="s">
+      <c r="H92" s="19" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G92" t="s">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G93" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="H92" s="16" t="s">
+      <c r="H93" s="19" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G93" t="s">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G94" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="H93" s="16" t="s">
+      <c r="H94" s="19" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G94" t="s">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G95" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="H94" s="16" t="s">
+      <c r="H95" s="19" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G95" t="s">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G96" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="H95" s="16" t="s">
+      <c r="H96" s="19" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G96" t="s">
+    <row r="97" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G97" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="H96" s="16" t="s">
+      <c r="H97" s="19" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="97" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G97" t="s">
+    <row r="98" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G98" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="H97" s="16" t="s">
+      <c r="H98" s="19" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="98" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G98" t="s">
+    <row r="99" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G99" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="H98" s="16" t="s">
+      <c r="H99" s="19" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="99" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G99" t="s">
+    <row r="100" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G100" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="H99" s="16" t="s">
+      <c r="H100" s="19" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="100" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G100" t="s">
+    <row r="101" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G101" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="H101" s="19" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="102" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G102" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="H100" s="16" t="s">
+      <c r="H102" s="19" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="103" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G103" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="H103" s="19" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="101" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G101" t="s">
-        <v>125</v>
-      </c>
-      <c r="H101" s="16" t="s">
+    <row r="104" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G104" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="H104" s="19" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="102" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G102" t="s">
-        <v>126</v>
-      </c>
-      <c r="H102" s="16" t="s">
+    <row r="105" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G105" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="H105" s="19" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="103" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G103" t="s">
-        <v>127</v>
-      </c>
-      <c r="H103" s="16" t="s">
+    <row r="106" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G106" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="H106" s="19" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="104" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G104" t="s">
-        <v>128</v>
-      </c>
-      <c r="H104" s="16" t="s">
+    <row r="107" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G107" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="H107" s="19" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="105" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G105" t="s">
-        <v>129</v>
-      </c>
-      <c r="H105" s="16" t="s">
+    <row r="108" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G108" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="H108" s="19" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="106" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G106" t="s">
-        <v>130</v>
-      </c>
-      <c r="H106" s="16" t="s">
+    <row r="109" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G109" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="H109" s="19" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="107" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G107" t="s">
-        <v>131</v>
-      </c>
-      <c r="H107" s="16" t="s">
+    <row r="110" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G110" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="H110" s="19" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="108" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G108" t="s">
-        <v>132</v>
-      </c>
-      <c r="H108" s="16" t="s">
+    <row r="111" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G111" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="H111" s="19" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="109" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G109" t="s">
-        <v>133</v>
-      </c>
-      <c r="H109" s="16" t="s">
+    <row r="112" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G112" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="H112" s="19" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="110" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G110" t="s">
-        <v>134</v>
-      </c>
-      <c r="H110" s="16" t="s">
+    <row r="113" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G113" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="H113" s="19" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="111" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G111" t="s">
-        <v>135</v>
-      </c>
-      <c r="H111" s="16" t="s">
+    <row r="114" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G114" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="H114" s="19" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="112" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G112" t="s">
-        <v>136</v>
-      </c>
-      <c r="H112" s="16" t="s">
+    <row r="115" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G115" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="H115" s="19" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="113" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G113" t="s">
-        <v>137</v>
-      </c>
-      <c r="H113" s="16" t="s">
+    <row r="116" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G116" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="H116" s="19" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="114" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G114" t="s">
-        <v>138</v>
-      </c>
-      <c r="H114" s="16" t="s">
+    <row r="117" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G117" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="H117" s="19" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="115" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G115" t="s">
-        <v>139</v>
-      </c>
-      <c r="H115" s="16" t="s">
+    <row r="118" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G118" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="H118" s="19" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="116" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G116" t="s">
-        <v>140</v>
-      </c>
-      <c r="H116" s="16" t="s">
+    <row r="119" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G119" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="H119" s="19" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="117" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G117" t="s">
-        <v>141</v>
-      </c>
-      <c r="H117" s="16" t="s">
+    <row r="120" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G120" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="H120" s="19" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="118" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G118" t="s">
-        <v>142</v>
-      </c>
-      <c r="H118" s="16" t="s">
+    <row r="121" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G121" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="H121" s="19" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="119" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G119" t="s">
-        <v>143</v>
-      </c>
-      <c r="H119" s="16" t="s">
+    <row r="122" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G122" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="H122" s="19" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="120" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G120" t="s">
-        <v>144</v>
-      </c>
-      <c r="H120" s="16" t="s">
+    <row r="123" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G123" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="H123" s="19" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="121" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G121" t="s">
-        <v>145</v>
-      </c>
-      <c r="H121" s="16" t="s">
+    <row r="124" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G124" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="H124" s="19" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="122" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G122" t="s">
-        <v>146</v>
-      </c>
-      <c r="H122" s="16" t="s">
+    <row r="125" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G125" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="H125" s="19" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="123" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G123" t="s">
-        <v>147</v>
-      </c>
-      <c r="H123" s="16" t="s">
+    <row r="126" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G126" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="H126" s="19" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="124" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G124" t="s">
-        <v>148</v>
-      </c>
-      <c r="H124" s="16" t="s">
+    <row r="127" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G127" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="H127" s="19" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="125" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G125" t="s">
-        <v>149</v>
-      </c>
-      <c r="H125" s="16" t="s">
+    <row r="128" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G128" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="H128" s="19" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="126" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G126" t="s">
-        <v>150</v>
-      </c>
-      <c r="H126" s="16" t="s">
+    <row r="129" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G129" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="H129" s="19" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="127" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G127" t="s">
-        <v>151</v>
-      </c>
-      <c r="H127" s="16" t="s">
+    <row r="130" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G130" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="H130" s="19" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="128" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G128" t="s">
-        <v>152</v>
-      </c>
-      <c r="H128" s="16" t="s">
+    <row r="131" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G131" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="H131" s="19" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="129" spans="7:9" x14ac:dyDescent="0.2">
-      <c r="G129" t="s">
-        <v>153</v>
-      </c>
-      <c r="H129" s="16" t="s">
+    <row r="132" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G132" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="H132" s="19" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="130" spans="7:9" x14ac:dyDescent="0.2">
-      <c r="G130" t="s">
-        <v>154</v>
-      </c>
-      <c r="H130" s="16" t="s">
+    <row r="133" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G133" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="H133" s="19" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="131" spans="7:9" x14ac:dyDescent="0.2">
-      <c r="G131" t="s">
-        <v>155</v>
-      </c>
-      <c r="H131" s="16" t="s">
+    <row r="134" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G134" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="H134" s="19" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="132" spans="7:9" x14ac:dyDescent="0.2">
-      <c r="G132" t="s">
-        <v>156</v>
-      </c>
-      <c r="H132" s="16" t="s">
+      <c r="I134" s="24"/>
+    </row>
+    <row r="135" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G135" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="H135" s="19" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="133" spans="7:9" x14ac:dyDescent="0.2">
-      <c r="G133" t="s">
-        <v>157</v>
-      </c>
-      <c r="H133" s="16" t="s">
+    <row r="136" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G136" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="H136" s="19" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="134" spans="7:9" x14ac:dyDescent="0.2">
-      <c r="G134" t="s">
-        <v>158</v>
-      </c>
-      <c r="H134" s="16" t="s">
+    <row r="137" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G137" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="H137" s="19" t="s">
         <v>395</v>
       </c>
-      <c r="I134" s="14"/>
-    </row>
-    <row r="135" spans="7:9" x14ac:dyDescent="0.2">
-      <c r="G135" t="s">
-        <v>159</v>
-      </c>
-      <c r="H135" s="16" t="s">
+    </row>
+    <row r="138" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G138" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="H138" s="19" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="136" spans="7:9" x14ac:dyDescent="0.2">
-      <c r="G136" t="s">
-        <v>160</v>
-      </c>
-      <c r="H136" s="16" t="s">
+    <row r="139" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G139" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="H139" s="19" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="137" spans="7:9" x14ac:dyDescent="0.2">
-      <c r="G137" t="s">
-        <v>161</v>
-      </c>
-      <c r="H137" s="16" t="s">
+    <row r="140" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G140" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="H140" s="19" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="138" spans="7:9" x14ac:dyDescent="0.2">
-      <c r="G138" t="s">
-        <v>162</v>
-      </c>
-      <c r="H138" s="16" t="s">
+    <row r="141" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G141" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="H141" s="19" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="139" spans="7:9" x14ac:dyDescent="0.2">
-      <c r="G139" t="s">
-        <v>163</v>
-      </c>
-      <c r="H139" s="16" t="s">
+    <row r="142" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G142" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="H142" s="19" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="140" spans="7:9" x14ac:dyDescent="0.2">
-      <c r="G140" t="s">
-        <v>164</v>
-      </c>
-      <c r="H140" s="16" t="s">
+    <row r="143" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G143" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="H143" s="19" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="141" spans="7:9" x14ac:dyDescent="0.2">
-      <c r="G141" t="s">
-        <v>165</v>
-      </c>
-      <c r="H141" s="16" t="s">
+    <row r="144" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G144" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="H144" s="19" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="142" spans="7:9" x14ac:dyDescent="0.2">
-      <c r="G142" t="s">
-        <v>166</v>
-      </c>
-      <c r="H142" s="16" t="s">
+    <row r="145" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G145" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="H145" s="19" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="143" spans="7:9" x14ac:dyDescent="0.2">
-      <c r="G143" t="s">
-        <v>167</v>
-      </c>
-      <c r="H143" s="16" t="s">
+    <row r="146" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G146" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="H146" s="19" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="144" spans="7:9" x14ac:dyDescent="0.2">
-      <c r="G144" t="s">
-        <v>168</v>
-      </c>
-      <c r="H144" s="16" t="s">
+    <row r="147" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G147" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="H147" s="19" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="145" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G145" t="s">
-        <v>169</v>
-      </c>
-      <c r="H145" s="16" t="s">
+    <row r="148" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G148" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="H148" s="19" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="146" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G146" t="s">
-        <v>170</v>
-      </c>
-      <c r="H146" s="16" t="s">
+    <row r="149" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G149" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="H149" s="19" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="147" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G147" t="s">
-        <v>171</v>
-      </c>
-      <c r="H147" s="16" t="s">
+    <row r="150" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G150" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="H150" s="19" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="148" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G148" t="s">
-        <v>172</v>
-      </c>
-      <c r="H148" s="16" t="s">
+    <row r="151" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G151" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="H151" s="19" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="149" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G149" t="s">
-        <v>173</v>
-      </c>
-      <c r="H149" s="16" t="s">
+    <row r="152" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G152" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="H152" s="19" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="150" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G150" t="s">
-        <v>174</v>
-      </c>
-      <c r="H150" s="16" t="s">
+    <row r="153" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G153" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="H153" s="19" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="151" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G151" t="s">
-        <v>175</v>
-      </c>
-      <c r="H151" s="16" t="s">
+    <row r="154" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G154" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="H154" s="19" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="152" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G152" t="s">
-        <v>176</v>
-      </c>
-      <c r="H152" s="16" t="s">
+    <row r="155" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G155" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="H155" s="19" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="153" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G153" t="s">
-        <v>177</v>
-      </c>
-      <c r="H153" s="16" t="s">
+    <row r="156" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G156" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="H156" s="19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="157" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G157" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="H157" s="19" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="154" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G154" t="s">
-        <v>178</v>
-      </c>
-      <c r="H154" s="16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="155" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G155" t="s">
-        <v>179</v>
-      </c>
-      <c r="H155" s="16" t="s">
+    <row r="158" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G158" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="H158" s="19" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="156" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G156" t="s">
-        <v>180</v>
-      </c>
-      <c r="H156" s="16" t="s">
+    <row r="159" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G159" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="H159" s="19" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="157" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G157" t="s">
-        <v>181</v>
-      </c>
-      <c r="H157" s="16" t="s">
+    <row r="160" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G160" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="H160" s="19" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="158" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G158" t="s">
-        <v>182</v>
-      </c>
-      <c r="H158" s="16" t="s">
+    <row r="161" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G161" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="H161" s="19" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="159" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G159" t="s">
-        <v>183</v>
-      </c>
-      <c r="H159" s="16" t="s">
+    <row r="162" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G162" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="H162" s="19" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="160" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G160" t="s">
-        <v>184</v>
-      </c>
-      <c r="H160" s="16" t="s">
+    <row r="163" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G163" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="H163" s="19" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="161" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G161" t="s">
-        <v>185</v>
-      </c>
-      <c r="H161" s="16" t="s">
+    <row r="164" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G164" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="H164" s="19" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="162" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G162" t="s">
-        <v>186</v>
-      </c>
-      <c r="H162" s="16" t="s">
+    <row r="165" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G165" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="H165" s="19" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="163" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G163" t="s">
-        <v>187</v>
-      </c>
-      <c r="H163" s="16" t="s">
+    <row r="166" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G166" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="H166" s="19" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="164" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G164" t="s">
-        <v>188</v>
-      </c>
-      <c r="H164" s="16" t="s">
+    <row r="167" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G167" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="H167" s="19" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="165" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G165" t="s">
-        <v>189</v>
-      </c>
-      <c r="H165" s="16" t="s">
+    <row r="168" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G168" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="H168" s="19" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="166" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G166" t="s">
-        <v>190</v>
-      </c>
-      <c r="H166" s="16" t="s">
+    <row r="169" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G169" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="H169" s="19" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="167" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G167" t="s">
-        <v>191</v>
-      </c>
-      <c r="H167" s="16" t="s">
+    <row r="170" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G170" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="H170" s="19" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="168" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G168" t="s">
-        <v>192</v>
-      </c>
-      <c r="H168" s="16" t="s">
+    <row r="171" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G171" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="H171" s="19" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="169" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G169" t="s">
-        <v>193</v>
-      </c>
-      <c r="H169" s="16" t="s">
+    <row r="172" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G172" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="H172" s="19" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="170" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G170" t="s">
-        <v>194</v>
-      </c>
-      <c r="H170" s="16" t="s">
+    <row r="173" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G173" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="H173" s="19" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="171" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G171" t="s">
-        <v>195</v>
-      </c>
-      <c r="H171" s="16" t="s">
+    <row r="174" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G174" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="H174" s="19" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="172" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G172" t="s">
-        <v>196</v>
-      </c>
-      <c r="H172" s="16" t="s">
+    <row r="175" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G175" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="H175" s="19" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="173" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G173" t="s">
-        <v>197</v>
-      </c>
-      <c r="H173" s="16" t="s">
+    <row r="176" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G176" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="H176" s="19" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="174" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G174" t="s">
-        <v>198</v>
-      </c>
-      <c r="H174" s="16" t="s">
+    <row r="177" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G177" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="H177" s="19" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="175" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G175" t="s">
-        <v>199</v>
-      </c>
-      <c r="H175" s="16" t="s">
+    <row r="178" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G178" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="H178" s="19" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="176" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G176" t="s">
-        <v>200</v>
-      </c>
-      <c r="H176" s="16" t="s">
+    <row r="179" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G179" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="H179" s="19" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="177" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G177" t="s">
-        <v>201</v>
-      </c>
-      <c r="H177" s="16" t="s">
+    <row r="180" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G180" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="H180" s="19" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="178" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G178" t="s">
-        <v>202</v>
-      </c>
-      <c r="H178" s="16" t="s">
+    <row r="181" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G181" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="H181" s="19" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="179" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G179" t="s">
-        <v>203</v>
-      </c>
-      <c r="H179" s="16" t="s">
+    <row r="182" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G182" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="H182" s="19" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="180" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G180" t="s">
-        <v>204</v>
-      </c>
-      <c r="H180" s="16" t="s">
+    <row r="183" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G183" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="H183" s="19" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="181" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G181" t="s">
-        <v>205</v>
-      </c>
-      <c r="H181" s="16" t="s">
+    <row r="184" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G184" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="H184" s="19" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="182" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G182" t="s">
-        <v>206</v>
-      </c>
-      <c r="H182" s="16" t="s">
+    <row r="185" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G185" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="H185" s="19" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="183" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G183" t="s">
-        <v>207</v>
-      </c>
-      <c r="H183" s="16" t="s">
+    <row r="186" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G186" s="20" t="s">
+        <v>208</v>
+      </c>
+      <c r="H186" s="19" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="184" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G184" t="s">
-        <v>208</v>
-      </c>
-      <c r="H184" s="16" t="s">
+    <row r="187" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G187" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="H187" s="19" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="185" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G185" t="s">
-        <v>209</v>
-      </c>
-      <c r="H185" s="16" t="s">
+    <row r="188" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G188" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="H188" s="19" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="186" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G186" t="s">
-        <v>210</v>
-      </c>
-      <c r="H186" s="16" t="s">
+    <row r="189" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G189" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="H189" s="19" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="187" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G187" t="s">
-        <v>211</v>
-      </c>
-      <c r="H187" s="16" t="s">
+    <row r="190" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G190" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="H190" s="19" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="188" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G188" t="s">
-        <v>212</v>
-      </c>
-      <c r="H188" s="16" t="s">
+    <row r="191" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G191" s="20" t="s">
+        <v>213</v>
+      </c>
+      <c r="H191" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="192" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G192" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="H192" s="19" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="189" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G189" t="s">
-        <v>213</v>
-      </c>
-      <c r="H189" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="190" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G190" t="s">
-        <v>214</v>
-      </c>
-      <c r="H190" s="16" t="s">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G193" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="H193" s="19" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="191" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G191" t="s">
-        <v>215</v>
-      </c>
-      <c r="H191" s="16" t="s">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G194" s="20" t="s">
+        <v>216</v>
+      </c>
+      <c r="H194" s="19" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="192" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G192" t="s">
-        <v>216</v>
-      </c>
-      <c r="H192" s="16" t="s">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G195" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="H195" s="19" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="193" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="G193" t="s">
-        <v>217</v>
-      </c>
-      <c r="H193" s="16" t="s">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G196" s="20" t="s">
+        <v>218</v>
+      </c>
+      <c r="H196" s="19" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="194" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="G194" t="s">
-        <v>218</v>
-      </c>
-      <c r="H194" s="16" t="s">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A197" s="21"/>
+      <c r="B197" s="22"/>
+      <c r="C197" s="22"/>
+      <c r="D197" s="22"/>
+      <c r="E197" s="22"/>
+      <c r="F197" s="22"/>
+      <c r="G197" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="H197" s="19" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="195" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="G195" t="s">
-        <v>219</v>
-      </c>
-      <c r="H195" s="16" t="s">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A198" s="21"/>
+      <c r="B198" s="22"/>
+      <c r="C198" s="22"/>
+      <c r="D198" s="22"/>
+      <c r="E198" s="22"/>
+      <c r="F198" s="22"/>
+      <c r="G198" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="H198" s="19" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="196" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="G196" t="s">
-        <v>220</v>
-      </c>
-      <c r="H196" s="16" t="s">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A199" s="21"/>
+      <c r="B199" s="22"/>
+      <c r="C199" s="22"/>
+      <c r="D199" s="22"/>
+      <c r="E199" s="22"/>
+      <c r="F199" s="22"/>
+      <c r="G199" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="H199" s="19" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="197" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="G197" t="s">
-        <v>221</v>
-      </c>
-      <c r="H197" s="16" t="s">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A200" s="21"/>
+      <c r="B200" s="22"/>
+      <c r="C200" s="22"/>
+      <c r="D200" s="22"/>
+      <c r="E200" s="22"/>
+      <c r="F200" s="22"/>
+      <c r="G200" s="20" t="s">
+        <v>222</v>
+      </c>
+      <c r="H200" s="19" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="198" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="G198" t="s">
-        <v>222</v>
-      </c>
-      <c r="H198" s="16" t="s">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A201" s="21"/>
+      <c r="B201" s="22"/>
+      <c r="C201" s="22"/>
+      <c r="D201" s="22"/>
+      <c r="E201" s="22"/>
+      <c r="F201" s="22"/>
+      <c r="G201" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="H201" s="19" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="199" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="G199" t="s">
-        <v>223</v>
-      </c>
-      <c r="H199" s="16" t="s">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A202" s="21"/>
+      <c r="B202" s="22"/>
+      <c r="C202" s="22"/>
+      <c r="D202" s="22"/>
+      <c r="E202" s="22"/>
+      <c r="F202" s="22"/>
+      <c r="G202" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="H202" s="19" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="200" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="F200" s="17"/>
-      <c r="G200" t="s">
-        <v>224</v>
-      </c>
-      <c r="H200" s="16" t="s">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A203" s="21"/>
+      <c r="B203" s="22"/>
+      <c r="C203" s="22"/>
+      <c r="D203" s="22"/>
+      <c r="E203" s="22"/>
+      <c r="F203" s="22"/>
+      <c r="G203" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="H203" s="19" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="201" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="G201" t="s">
-        <v>225</v>
-      </c>
-      <c r="H201" s="16" t="s">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A204" s="21"/>
+      <c r="B204" s="22"/>
+      <c r="C204" s="22"/>
+      <c r="D204" s="22"/>
+      <c r="E204" s="22"/>
+      <c r="F204" s="22"/>
+      <c r="G204" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="H204" s="19" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="202" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="G202" t="s">
-        <v>226</v>
-      </c>
-      <c r="H202" s="16" t="s">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A205" s="21"/>
+      <c r="B205" s="22"/>
+      <c r="C205" s="22"/>
+      <c r="D205" s="22"/>
+      <c r="E205" s="22"/>
+      <c r="F205" s="22"/>
+      <c r="G205" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="H205" s="19" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="203" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="G203" t="s">
-        <v>227</v>
-      </c>
-      <c r="H203" s="16" t="s">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A206" s="21"/>
+      <c r="B206" s="22"/>
+      <c r="C206" s="22"/>
+      <c r="D206" s="22"/>
+      <c r="E206" s="22"/>
+      <c r="F206" s="22"/>
+      <c r="G206" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="H206" s="19" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="204" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="G204" t="s">
-        <v>228</v>
-      </c>
-      <c r="H204" s="16" t="s">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A207" s="21"/>
+      <c r="B207" s="22"/>
+      <c r="C207" s="22"/>
+      <c r="D207" s="22"/>
+      <c r="E207" s="22"/>
+      <c r="F207" s="22"/>
+      <c r="G207" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="H207" s="19" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="205" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="G205" t="s">
-        <v>229</v>
-      </c>
-      <c r="H205" s="16" t="s">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A208" s="21"/>
+      <c r="B208" s="22"/>
+      <c r="C208" s="22"/>
+      <c r="D208" s="23"/>
+      <c r="E208" s="22"/>
+      <c r="F208" s="22"/>
+      <c r="G208" s="20" t="s">
+        <v>230</v>
+      </c>
+      <c r="H208" s="19" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="206" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="G206" t="s">
-        <v>230</v>
-      </c>
-      <c r="H206" s="16" t="s">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A209" s="21"/>
+      <c r="B209" s="22"/>
+      <c r="C209" s="22"/>
+      <c r="D209" s="22"/>
+      <c r="E209" s="22"/>
+      <c r="F209" s="22"/>
+      <c r="G209" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="H209" s="19" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="207" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="G207" t="s">
-        <v>231</v>
-      </c>
-      <c r="H207" s="16" t="s">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A210" s="21"/>
+      <c r="B210" s="22"/>
+      <c r="C210" s="22"/>
+      <c r="D210" s="22"/>
+      <c r="E210" s="22"/>
+      <c r="F210" s="22"/>
+      <c r="G210" s="18" t="s">
+        <v>232</v>
+      </c>
+      <c r="H210" s="19" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="208" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C208" t="s">
-        <v>123</v>
-      </c>
-      <c r="D208" s="16" t="s">
-        <v>360</v>
-      </c>
-      <c r="G208" t="s">
-        <v>232</v>
-      </c>
-      <c r="H208" s="16" t="s">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A211" s="21"/>
+      <c r="B211" s="22"/>
+      <c r="C211" s="22"/>
+      <c r="D211" s="22"/>
+      <c r="E211" s="22"/>
+      <c r="F211" s="22"/>
+      <c r="G211" s="20" t="s">
+        <v>233</v>
+      </c>
+      <c r="H211" s="19" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="209" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G209" t="s">
-        <v>233</v>
-      </c>
-      <c r="H209" s="16" t="s">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A212" s="21"/>
+      <c r="B212" s="22"/>
+      <c r="C212" s="22"/>
+      <c r="D212" s="22"/>
+      <c r="E212" s="22"/>
+      <c r="F212" s="22"/>
+      <c r="G212" s="20" t="s">
+        <v>234</v>
+      </c>
+      <c r="H212" s="19" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G213" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="H213" s="19" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="210" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G210" t="s">
-        <v>234</v>
-      </c>
-      <c r="H210" s="16" t="s">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G214" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="H214" s="19" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="211" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G211" t="s">
-        <v>235</v>
-      </c>
-      <c r="H211" s="16" t="s">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G215" s="20" t="s">
+        <v>237</v>
+      </c>
+      <c r="H215" s="19" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G216" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="H216" s="19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G217" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="H217" s="19" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="212" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G212" t="s">
-        <v>236</v>
-      </c>
-      <c r="H212" s="16" t="s">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G218" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="H218" s="19" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="219" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G219" s="20" t="s">
+        <v>241</v>
+      </c>
+      <c r="H219" s="19" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G220" s="20" t="s">
+        <v>242</v>
+      </c>
+      <c r="H220" s="19" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G221" s="20" t="s">
+        <v>243</v>
+      </c>
+      <c r="H221" s="19" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="213" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G213" t="s">
-        <v>237</v>
-      </c>
-      <c r="H213" s="16" t="s">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G222" s="20" t="s">
+        <v>244</v>
+      </c>
+      <c r="H222" s="19" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G223" s="20" t="s">
+        <v>245</v>
+      </c>
+      <c r="H223" s="19" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="224" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G224" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="H224" s="19" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="214" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G214" t="s">
-        <v>238</v>
-      </c>
-      <c r="H214" s="16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="215" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G215" t="s">
-        <v>239</v>
-      </c>
-      <c r="H215" s="16" t="s">
+    <row r="225" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G225" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="H225" s="19" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="216" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G216" t="s">
-        <v>240</v>
-      </c>
-      <c r="H216" s="16" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="217" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G217" t="s">
-        <v>241</v>
-      </c>
-      <c r="H217" s="16" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="218" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G218" t="s">
-        <v>242</v>
-      </c>
-      <c r="H218" s="16" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="219" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G219" t="s">
-        <v>243</v>
-      </c>
-      <c r="H219" s="16" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="220" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G220" t="s">
-        <v>244</v>
-      </c>
-      <c r="H220" s="16" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="221" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G221" t="s">
-        <v>245</v>
-      </c>
-      <c r="H221" s="16" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="222" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G222" t="s">
-        <v>246</v>
-      </c>
-      <c r="H222" s="16" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="223" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G223" t="s">
-        <v>247</v>
-      </c>
-      <c r="H223" s="16" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="224" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G224" t="s">
+    <row r="226" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G226" s="20" t="s">
         <v>248</v>
       </c>
-      <c r="H224" s="16" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="225" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="G225" t="s">
+      <c r="H226" s="25" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="227" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G227" s="20" t="s">
         <v>249</v>
       </c>
-      <c r="H225" s="16" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="226" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="G226" t="s">
+      <c r="H227" s="25" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="228" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G228" s="20" t="s">
         <v>250</v>
       </c>
-      <c r="H226" s="16" t="s">
+      <c r="H228" s="25" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="229" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G229" s="20" t="s">
+        <v>251</v>
+      </c>
+      <c r="H229" s="25" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="230" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G230" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="H230" s="25" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="231" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G231" s="20" t="s">
+        <v>253</v>
+      </c>
+      <c r="H231" s="25" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="232" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G232" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="H232" s="25" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="233" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G233" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="H233" s="25" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="234" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G234" s="20" t="s">
+        <v>256</v>
+      </c>
+      <c r="H234" s="25" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="235" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G235" s="20" t="s">
+        <v>257</v>
+      </c>
+      <c r="H235" s="25" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="236" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G236" s="20" t="s">
+        <v>258</v>
+      </c>
+      <c r="H236" s="25" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="237" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G237" s="20" t="s">
+        <v>259</v>
+      </c>
+      <c r="H237" s="25" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="238" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G238" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="H238" s="25" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="239" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G239" s="20" t="s">
+        <v>261</v>
+      </c>
+      <c r="H239" s="25" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="240" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G240" s="20" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="227" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="G227" t="s">
-        <v>251</v>
-      </c>
-      <c r="H227" s="16" t="s">
+      <c r="H240" s="25" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="241" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G241" s="20" t="s">
         <v>485</v>
       </c>
-    </row>
-    <row r="228" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="G228" t="s">
-        <v>252</v>
-      </c>
-      <c r="H228" s="16" t="s">
+      <c r="H241" s="25" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="242" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G242" s="20" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="229" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="G229" t="s">
-        <v>253</v>
-      </c>
-      <c r="H229" s="16" t="s">
+      <c r="H242" s="25" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="243" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G243" s="20" t="s">
         <v>487</v>
       </c>
-    </row>
-    <row r="230" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="G230" t="s">
-        <v>254</v>
-      </c>
-      <c r="H230" s="16" t="s">
+      <c r="H243" s="25" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="244" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G244" s="20" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="231" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="G231" t="s">
-        <v>255</v>
-      </c>
-      <c r="H231" s="16" t="s">
+      <c r="H244" s="25" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="245" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G245" s="20" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="232" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="G232" t="s">
-        <v>256</v>
-      </c>
-      <c r="H232" s="16" t="s">
+      <c r="H245" s="25" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="246" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G246" s="20" t="s">
         <v>490</v>
       </c>
-    </row>
-    <row r="233" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="G233" t="s">
-        <v>257</v>
-      </c>
-      <c r="H233" s="16" t="s">
+      <c r="H246" s="25" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="247" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G247" s="20" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="234" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="G234" t="s">
-        <v>123</v>
-      </c>
-      <c r="H234" s="16" t="s">
+      <c r="H247" s="25" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="248" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G248" s="20" t="s">
+        <v>492</v>
+      </c>
+      <c r="H248" s="25" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="249" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G249" s="20" t="s">
+        <v>493</v>
+      </c>
+      <c r="H249" s="25" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="250" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G250" s="20" t="s">
+        <v>494</v>
+      </c>
+      <c r="H250" s="26" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="251" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G251" t="s">
+        <v>495</v>
+      </c>
+      <c r="H251" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="252" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G252" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="235" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="G235" t="s">
-        <v>258</v>
-      </c>
-      <c r="H235" s="16" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="236" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="G236" t="s">
-        <v>259</v>
-      </c>
-      <c r="H236" s="16" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="237" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="G237" t="s">
-        <v>260</v>
-      </c>
-      <c r="H237" s="16" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="238" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="G238" t="s">
-        <v>261</v>
-      </c>
-      <c r="H238" s="16" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="240" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C240" s="18"/>
-      <c r="D240" s="18"/>
-      <c r="E240" s="18"/>
-      <c r="F240" s="18"/>
-      <c r="I240" s="18"/>
-      <c r="J240" s="18"/>
-      <c r="K240" s="18"/>
-    </row>
-    <row r="241" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C241" s="18"/>
-      <c r="D241" s="18"/>
-      <c r="E241" s="18"/>
-      <c r="F241" s="18"/>
-      <c r="I241" s="18"/>
-      <c r="J241" s="18"/>
-      <c r="K241" s="18"/>
-    </row>
-    <row r="242" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C242" s="18"/>
-      <c r="D242" s="18"/>
-      <c r="E242" s="18"/>
-      <c r="F242" s="18"/>
-      <c r="I242" s="18"/>
-      <c r="J242" s="18"/>
-      <c r="K242" s="18"/>
-    </row>
-    <row r="243" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C243" s="18"/>
-      <c r="D243" s="18"/>
-      <c r="E243" s="18"/>
-      <c r="F243" s="18"/>
-      <c r="G243" s="18"/>
-      <c r="H243" s="18"/>
-      <c r="I243" s="18"/>
-      <c r="J243" s="18"/>
-      <c r="K243" s="18"/>
-    </row>
-    <row r="244" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C244" s="18"/>
-      <c r="D244" s="18"/>
-      <c r="E244" s="18"/>
-      <c r="F244" s="18"/>
-      <c r="G244" s="18"/>
-      <c r="H244" s="18"/>
-      <c r="I244" s="18"/>
-      <c r="J244" s="18"/>
-      <c r="K244" s="18"/>
-    </row>
-    <row r="245" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C245" s="18"/>
-      <c r="D245" s="18"/>
-      <c r="E245" s="18"/>
-      <c r="F245" s="18"/>
-      <c r="G245" s="18"/>
-      <c r="H245" s="18"/>
-      <c r="I245" s="18"/>
-      <c r="J245" s="18"/>
-      <c r="K245" s="18"/>
-    </row>
-    <row r="246" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C246" s="18"/>
-      <c r="D246" s="18"/>
-      <c r="E246" s="18"/>
-      <c r="F246" s="18"/>
-      <c r="G246" s="18"/>
-      <c r="H246" s="18"/>
-      <c r="I246" s="18"/>
-      <c r="J246" s="18"/>
-      <c r="K246" s="18"/>
-    </row>
-    <row r="247" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C247" s="18"/>
-      <c r="D247" s="18"/>
-      <c r="E247" s="18"/>
-      <c r="F247" s="18"/>
-      <c r="G247" s="18"/>
-      <c r="H247" s="18"/>
-      <c r="I247" s="18"/>
-      <c r="J247" s="18"/>
-      <c r="K247" s="18"/>
-    </row>
-    <row r="248" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C248" s="18"/>
-      <c r="D248" s="18"/>
-      <c r="E248" s="18"/>
-      <c r="F248" s="18"/>
-      <c r="G248" s="19"/>
-      <c r="H248" s="18"/>
-      <c r="I248" s="18"/>
-      <c r="J248" s="18"/>
-      <c r="K248" s="18"/>
-    </row>
-    <row r="249" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C249" s="18"/>
-      <c r="D249" s="18"/>
-      <c r="E249" s="18"/>
-      <c r="F249" s="18"/>
-      <c r="G249" s="19"/>
-      <c r="H249" s="18"/>
-      <c r="I249" s="18"/>
-      <c r="J249" s="18"/>
-      <c r="K249" s="18"/>
-    </row>
-    <row r="250" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C250" s="18"/>
-      <c r="D250" s="18"/>
-      <c r="E250" s="18"/>
-      <c r="F250" s="18"/>
-      <c r="G250" s="19"/>
-      <c r="H250" s="18"/>
-      <c r="I250" s="18"/>
-      <c r="J250" s="18"/>
-      <c r="K250" s="18"/>
-    </row>
-    <row r="251" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C251" s="18"/>
-      <c r="D251" s="18"/>
-      <c r="E251" s="18"/>
-      <c r="F251" s="18"/>
-      <c r="G251" s="19"/>
-      <c r="H251" s="18"/>
-      <c r="I251" s="18"/>
-      <c r="J251" s="18"/>
-      <c r="K251" s="18"/>
-    </row>
-    <row r="252" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C252" s="18"/>
-      <c r="D252" s="18"/>
-      <c r="E252" s="18"/>
-      <c r="F252" s="18"/>
-      <c r="G252" s="19"/>
-      <c r="H252" s="18"/>
-      <c r="I252" s="18"/>
-      <c r="J252" s="18"/>
-      <c r="K252" s="18"/>
-    </row>
-    <row r="253" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C253" s="18"/>
-      <c r="D253" s="18"/>
-      <c r="E253" s="18"/>
-      <c r="F253" s="18"/>
-      <c r="G253" s="19"/>
-      <c r="H253" s="20"/>
-      <c r="I253" s="18"/>
-      <c r="J253" s="18"/>
-      <c r="K253" s="18"/>
-    </row>
-    <row r="254" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C254" s="18"/>
-      <c r="D254" s="18"/>
-      <c r="E254" s="18"/>
-      <c r="F254" s="18"/>
-      <c r="G254" s="19"/>
-      <c r="H254" s="20"/>
-      <c r="I254" s="20"/>
-      <c r="J254" s="20"/>
-      <c r="K254" s="18"/>
-    </row>
-    <row r="255" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C255" s="18"/>
-      <c r="D255" s="18"/>
-      <c r="E255" s="18"/>
-      <c r="F255" s="18"/>
-      <c r="G255" s="19"/>
-      <c r="H255" s="20"/>
-      <c r="I255" s="20"/>
-      <c r="J255" s="20"/>
-      <c r="K255" s="18"/>
-    </row>
-    <row r="256" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C256" s="18"/>
-      <c r="D256" s="18"/>
-      <c r="E256" s="18"/>
-      <c r="F256" s="18"/>
-      <c r="G256" s="19"/>
-      <c r="H256" s="20"/>
-      <c r="I256" s="20"/>
-      <c r="J256" s="20"/>
-      <c r="K256" s="18"/>
-    </row>
-    <row r="257" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C257" s="18"/>
-      <c r="D257" s="18"/>
-      <c r="E257" s="18"/>
-      <c r="F257" s="18"/>
-      <c r="G257" s="19"/>
-      <c r="H257" s="20"/>
-      <c r="I257" s="21"/>
-      <c r="J257" s="20"/>
-      <c r="K257" s="18"/>
-    </row>
-    <row r="258" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C258" s="18"/>
-      <c r="D258" s="18"/>
-      <c r="E258" s="18"/>
-      <c r="F258" s="18"/>
-      <c r="G258" s="19"/>
-      <c r="H258" s="20"/>
-      <c r="I258" s="22"/>
-      <c r="J258" s="20"/>
-      <c r="K258" s="18"/>
-    </row>
-    <row r="259" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C259" s="18"/>
-      <c r="D259" s="18"/>
-      <c r="E259" s="18"/>
-      <c r="F259" s="18"/>
-      <c r="G259" s="19"/>
-      <c r="H259" s="20"/>
-      <c r="I259" s="23"/>
-      <c r="J259" s="20"/>
-      <c r="K259" s="18"/>
-    </row>
-    <row r="260" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C260" s="18"/>
-      <c r="D260" s="18"/>
-      <c r="E260" s="18"/>
-      <c r="F260" s="18"/>
-      <c r="G260" s="18"/>
-      <c r="H260" s="20"/>
-      <c r="I260" s="23"/>
-      <c r="J260" s="20"/>
-      <c r="K260" s="18"/>
-    </row>
-    <row r="261" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C261" s="18"/>
-      <c r="D261" s="18"/>
-      <c r="E261" s="18"/>
-      <c r="F261" s="18"/>
-      <c r="G261" s="18"/>
-      <c r="H261" s="20"/>
-      <c r="I261" s="20"/>
-      <c r="J261" s="20"/>
-      <c r="K261" s="18"/>
-    </row>
-    <row r="262" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C262" s="18"/>
-      <c r="D262" s="18"/>
-      <c r="E262" s="18"/>
-      <c r="F262" s="18"/>
-      <c r="H262" s="24"/>
-      <c r="I262" s="20"/>
-      <c r="J262" s="20"/>
-      <c r="K262" s="18"/>
-    </row>
-    <row r="263" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="I263" s="24"/>
-      <c r="J263" s="24"/>
+      <c r="H252" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="253" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G253" t="s">
+        <v>524</v>
+      </c>
+      <c r="H253" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="254" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G254" t="s">
+        <v>526</v>
+      </c>
+      <c r="H254" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="255" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G255" s="1"/>
+    </row>
+    <row r="256" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G256" s="1"/>
+    </row>
+    <row r="257" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G257" s="1"/>
+      <c r="I257" s="15"/>
+    </row>
+    <row r="258" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G258" s="1"/>
+      <c r="I258" s="16"/>
+    </row>
+    <row r="259" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G259" s="1"/>
+      <c r="I259" s="17"/>
+    </row>
+    <row r="260" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="I260" s="17"/>
     </row>
     <row r="5455" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5455" s="4"/>

</xml_diff>